<commit_message>
wrote more; made a loadAll function to load all dataframes; made more graphs; started a script for stats & data summaries
</commit_message>
<xml_diff>
--- a/Sheets/datasetOverview.xlsx
+++ b/Sheets/datasetOverview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="1640" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="197">
   <si>
     <t>ID</t>
   </si>
@@ -586,6 +586,30 @@
   </si>
   <si>
     <t>McPherson Range, Australia</t>
+  </si>
+  <si>
+    <t>GenPeak</t>
+  </si>
+  <si>
+    <t>GenPeakEl</t>
+  </si>
+  <si>
+    <t>mostDivGenPeak</t>
+  </si>
+  <si>
+    <t>mostDivGenPeakEl</t>
+  </si>
+  <si>
+    <t>SFPeak</t>
+  </si>
+  <si>
+    <t>SFPeakEl</t>
+  </si>
+  <si>
+    <t>mostDivSFPeak</t>
+  </si>
+  <si>
+    <t>mostDivSFPeakEl</t>
   </si>
 </sst>
 </file>
@@ -1058,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN21"/>
+  <dimension ref="A1:AV21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AO8" sqref="AO8:AV11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1072,7 +1096,7 @@
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:48">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1193,8 +1217,32 @@
       <c r="AN1" t="s">
         <v>38</v>
       </c>
+      <c r="AO1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>196</v>
+      </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:48">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1315,8 +1363,32 @@
       <c r="AN2" t="s">
         <v>164</v>
       </c>
+      <c r="AO2">
+        <v>28</v>
+      </c>
+      <c r="AP2">
+        <v>1800</v>
+      </c>
+      <c r="AQ2">
+        <v>39</v>
+      </c>
+      <c r="AR2">
+        <v>1800</v>
+      </c>
+      <c r="AS2">
+        <v>6</v>
+      </c>
+      <c r="AT2">
+        <v>1800</v>
+      </c>
+      <c r="AU2">
+        <v>65</v>
+      </c>
+      <c r="AV2">
+        <v>1800</v>
+      </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:48">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1437,8 +1509,32 @@
       <c r="AN3" t="s">
         <v>164</v>
       </c>
+      <c r="AO3">
+        <v>22</v>
+      </c>
+      <c r="AP3">
+        <v>1300</v>
+      </c>
+      <c r="AQ3">
+        <v>30</v>
+      </c>
+      <c r="AR3">
+        <v>1300</v>
+      </c>
+      <c r="AS3">
+        <v>4</v>
+      </c>
+      <c r="AT3">
+        <v>800</v>
+      </c>
+      <c r="AU3">
+        <v>53</v>
+      </c>
+      <c r="AV3">
+        <v>1300</v>
+      </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:48">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1559,8 +1655,32 @@
       <c r="AN4" t="s">
         <v>165</v>
       </c>
+      <c r="AO4">
+        <v>27</v>
+      </c>
+      <c r="AP4">
+        <v>700</v>
+      </c>
+      <c r="AQ4">
+        <v>19</v>
+      </c>
+      <c r="AR4">
+        <v>600</v>
+      </c>
+      <c r="AS4">
+        <v>5</v>
+      </c>
+      <c r="AT4">
+        <v>100</v>
+      </c>
+      <c r="AU4">
+        <v>50</v>
+      </c>
+      <c r="AV4">
+        <v>600</v>
+      </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:48">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1681,8 +1801,32 @@
       <c r="AN5" t="s">
         <v>165</v>
       </c>
+      <c r="AO5">
+        <v>23</v>
+      </c>
+      <c r="AP5">
+        <v>1400</v>
+      </c>
+      <c r="AQ5">
+        <v>8</v>
+      </c>
+      <c r="AR5">
+        <v>1600</v>
+      </c>
+      <c r="AS5">
+        <v>6</v>
+      </c>
+      <c r="AT5">
+        <v>1400</v>
+      </c>
+      <c r="AU5">
+        <v>32</v>
+      </c>
+      <c r="AV5">
+        <v>1600</v>
+      </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:48">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1803,8 +1947,32 @@
       <c r="AN6" t="s">
         <v>164</v>
       </c>
+      <c r="AO6">
+        <v>23</v>
+      </c>
+      <c r="AP6">
+        <v>1400</v>
+      </c>
+      <c r="AQ6">
+        <v>31</v>
+      </c>
+      <c r="AR6">
+        <v>2100</v>
+      </c>
+      <c r="AS6">
+        <v>4</v>
+      </c>
+      <c r="AT6">
+        <v>1000</v>
+      </c>
+      <c r="AU6">
+        <v>54</v>
+      </c>
+      <c r="AV6">
+        <v>1900</v>
+      </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:48">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1926,7 +2094,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:48">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2047,8 +2215,32 @@
       <c r="AN8" t="s">
         <v>165</v>
       </c>
+      <c r="AO8">
+        <v>13</v>
+      </c>
+      <c r="AP8">
+        <v>250</v>
+      </c>
+      <c r="AQ8">
+        <v>8</v>
+      </c>
+      <c r="AR8">
+        <v>475</v>
+      </c>
+      <c r="AS8">
+        <v>4</v>
+      </c>
+      <c r="AT8">
+        <v>250</v>
+      </c>
+      <c r="AU8">
+        <v>20</v>
+      </c>
+      <c r="AV8">
+        <v>475</v>
+      </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:48">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2169,8 +2361,32 @@
       <c r="AN9" t="s">
         <v>165</v>
       </c>
+      <c r="AO9">
+        <v>26</v>
+      </c>
+      <c r="AP9">
+        <v>425</v>
+      </c>
+      <c r="AQ9">
+        <v>21</v>
+      </c>
+      <c r="AR9">
+        <v>875</v>
+      </c>
+      <c r="AS9">
+        <v>8</v>
+      </c>
+      <c r="AT9">
+        <v>425</v>
+      </c>
+      <c r="AU9">
+        <v>71</v>
+      </c>
+      <c r="AV9">
+        <v>825</v>
+      </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:48">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2291,8 +2507,32 @@
       <c r="AN10" t="s">
         <v>165</v>
       </c>
+      <c r="AO10">
+        <v>12</v>
+      </c>
+      <c r="AP10">
+        <v>800</v>
+      </c>
+      <c r="AQ10">
+        <v>7</v>
+      </c>
+      <c r="AR10">
+        <v>800</v>
+      </c>
+      <c r="AS10">
+        <v>6</v>
+      </c>
+      <c r="AT10">
+        <v>800</v>
+      </c>
+      <c r="AU10">
+        <v>13</v>
+      </c>
+      <c r="AV10">
+        <v>800</v>
+      </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:48">
       <c r="A11">
         <v>11</v>
       </c>
@@ -2413,8 +2653,32 @@
       <c r="AN11" t="s">
         <v>164</v>
       </c>
+      <c r="AO11">
+        <v>16</v>
+      </c>
+      <c r="AP11">
+        <v>800</v>
+      </c>
+      <c r="AQ11">
+        <v>14</v>
+      </c>
+      <c r="AR11">
+        <v>1000</v>
+      </c>
+      <c r="AS11">
+        <v>4</v>
+      </c>
+      <c r="AT11">
+        <v>600</v>
+      </c>
+      <c r="AU11">
+        <v>25</v>
+      </c>
+      <c r="AV11">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:48">
       <c r="A12">
         <v>12</v>
       </c>
@@ -2536,7 +2800,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:48">
       <c r="A13">
         <v>13</v>
       </c>
@@ -2657,8 +2921,32 @@
       <c r="AN13" t="s">
         <v>164</v>
       </c>
+      <c r="AO13">
+        <v>14</v>
+      </c>
+      <c r="AP13">
+        <v>400</v>
+      </c>
+      <c r="AQ13">
+        <v>14</v>
+      </c>
+      <c r="AR13">
+        <v>900</v>
+      </c>
+      <c r="AS13">
+        <v>4</v>
+      </c>
+      <c r="AT13">
+        <v>400</v>
+      </c>
+      <c r="AU13">
+        <v>22</v>
+      </c>
+      <c r="AV13">
+        <v>600</v>
+      </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:48">
       <c r="A14">
         <v>14</v>
       </c>
@@ -2779,8 +3067,32 @@
       <c r="AN14" t="s">
         <v>166</v>
       </c>
+      <c r="AO14">
+        <v>16</v>
+      </c>
+      <c r="AP14">
+        <v>440</v>
+      </c>
+      <c r="AQ14">
+        <v>6</v>
+      </c>
+      <c r="AR14">
+        <v>719</v>
+      </c>
+      <c r="AS14">
+        <v>6</v>
+      </c>
+      <c r="AT14">
+        <v>511</v>
+      </c>
+      <c r="AU14">
+        <v>16</v>
+      </c>
+      <c r="AV14">
+        <v>719</v>
+      </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:48">
       <c r="A15">
         <v>15</v>
       </c>
@@ -2901,8 +3213,32 @@
       <c r="AN15" t="s">
         <v>167</v>
       </c>
+      <c r="AO15">
+        <v>17</v>
+      </c>
+      <c r="AP15">
+        <v>1000</v>
+      </c>
+      <c r="AQ15">
+        <v>3</v>
+      </c>
+      <c r="AR15">
+        <v>800</v>
+      </c>
+      <c r="AS15">
+        <v>5</v>
+      </c>
+      <c r="AT15">
+        <v>1000</v>
+      </c>
+      <c r="AU15">
+        <v>12</v>
+      </c>
+      <c r="AV15">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:48">
       <c r="A16">
         <v>16</v>
       </c>
@@ -3023,8 +3359,32 @@
       <c r="AN16" t="s">
         <v>165</v>
       </c>
+      <c r="AO16">
+        <v>49</v>
+      </c>
+      <c r="AP16">
+        <v>300</v>
+      </c>
+      <c r="AQ16">
+        <v>10</v>
+      </c>
+      <c r="AR16">
+        <v>300</v>
+      </c>
+      <c r="AS16">
+        <v>10</v>
+      </c>
+      <c r="AT16">
+        <v>300</v>
+      </c>
+      <c r="AU16">
+        <v>47</v>
+      </c>
+      <c r="AV16">
+        <v>300</v>
+      </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:48">
       <c r="A17">
         <v>17</v>
       </c>
@@ -3145,8 +3505,32 @@
       <c r="AN17" t="s">
         <v>168</v>
       </c>
+      <c r="AO17">
+        <v>24</v>
+      </c>
+      <c r="AP17">
+        <v>100</v>
+      </c>
+      <c r="AQ17">
+        <v>9</v>
+      </c>
+      <c r="AR17">
+        <v>100</v>
+      </c>
+      <c r="AS17">
+        <v>5</v>
+      </c>
+      <c r="AT17">
+        <v>200</v>
+      </c>
+      <c r="AU17">
+        <v>36</v>
+      </c>
+      <c r="AV17">
+        <v>100</v>
+      </c>
     </row>
-    <row r="18" spans="1:40">
+    <row r="18" spans="1:48">
       <c r="A18">
         <v>18</v>
       </c>
@@ -3267,8 +3651,32 @@
       <c r="AN18" t="s">
         <v>165</v>
       </c>
+      <c r="AO18">
+        <v>61</v>
+      </c>
+      <c r="AP18">
+        <v>300</v>
+      </c>
+      <c r="AQ18">
+        <v>56</v>
+      </c>
+      <c r="AR18">
+        <v>500</v>
+      </c>
+      <c r="AS18">
+        <v>12</v>
+      </c>
+      <c r="AT18">
+        <v>50</v>
+      </c>
+      <c r="AU18">
+        <v>171</v>
+      </c>
+      <c r="AV18">
+        <v>500</v>
+      </c>
     </row>
-    <row r="19" spans="1:40">
+    <row r="19" spans="1:48">
       <c r="A19">
         <v>19</v>
       </c>
@@ -3390,7 +3798,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:40">
+    <row r="20" spans="1:48">
       <c r="A20">
         <v>20</v>
       </c>
@@ -3512,7 +3920,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:40">
+    <row r="21" spans="1:48">
       <c r="A21">
         <v>21</v>
       </c>
@@ -3632,6 +4040,30 @@
       </c>
       <c r="AN21" t="s">
         <v>169</v>
+      </c>
+      <c r="AO21">
+        <v>39</v>
+      </c>
+      <c r="AP21">
+        <v>300</v>
+      </c>
+      <c r="AQ21">
+        <v>16</v>
+      </c>
+      <c r="AR21">
+        <v>300</v>
+      </c>
+      <c r="AS21">
+        <v>7</v>
+      </c>
+      <c r="AT21">
+        <v>200</v>
+      </c>
+      <c r="AU21">
+        <v>71</v>
+      </c>
+      <c r="AV21">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrote more, added some graphs, reorganized citations list
</commit_message>
<xml_diff>
--- a/Sheets/datasetOverview.xlsx
+++ b/Sheets/datasetOverview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="-300" yWindow="0" windowWidth="10640" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="199">
   <si>
     <t>ID</t>
   </si>
@@ -610,6 +610,12 @@
   </si>
   <si>
     <t>mostDivSFPeakEl</t>
+  </si>
+  <si>
+    <t>seRng</t>
+  </si>
+  <si>
+    <t>mnRng</t>
   </si>
 </sst>
 </file>
@@ -1082,10 +1088,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV21"/>
+  <dimension ref="A1:AX21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AO8" sqref="AO8:AV11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AX21" sqref="AX21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1096,7 +1105,7 @@
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48">
+    <row r="1" spans="1:50">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1241,8 +1250,14 @@
       <c r="AV1" t="s">
         <v>196</v>
       </c>
+      <c r="AW1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>197</v>
+      </c>
     </row>
-    <row r="2" spans="1:48">
+    <row r="2" spans="1:50">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1387,8 +1402,14 @@
       <c r="AV2">
         <v>1800</v>
       </c>
+      <c r="AW2">
+        <v>924.63</v>
+      </c>
+      <c r="AX2">
+        <v>57.04</v>
+      </c>
     </row>
-    <row r="3" spans="1:48">
+    <row r="3" spans="1:50">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1533,8 +1554,14 @@
       <c r="AV3">
         <v>1300</v>
       </c>
+      <c r="AW3">
+        <v>951.24</v>
+      </c>
+      <c r="AX3">
+        <v>64</v>
+      </c>
     </row>
-    <row r="4" spans="1:48">
+    <row r="4" spans="1:50">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1679,8 +1706,14 @@
       <c r="AV4">
         <v>600</v>
       </c>
+      <c r="AW4">
+        <v>767.38</v>
+      </c>
+      <c r="AX4">
+        <v>52.04</v>
+      </c>
     </row>
-    <row r="5" spans="1:48">
+    <row r="5" spans="1:50">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1825,8 +1858,14 @@
       <c r="AV5">
         <v>1600</v>
       </c>
+      <c r="AW5">
+        <v>365.43</v>
+      </c>
+      <c r="AX5">
+        <v>34.83</v>
+      </c>
     </row>
-    <row r="6" spans="1:48">
+    <row r="6" spans="1:50">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1971,8 +2010,14 @@
       <c r="AV6">
         <v>1900</v>
       </c>
+      <c r="AW6">
+        <v>972.4</v>
+      </c>
+      <c r="AX6">
+        <v>50.75</v>
+      </c>
     </row>
-    <row r="7" spans="1:48">
+    <row r="7" spans="1:50">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2094,7 +2139,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:48">
+    <row r="8" spans="1:50">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2239,8 +2284,14 @@
       <c r="AV8">
         <v>475</v>
       </c>
+      <c r="AW8">
+        <v>247.12</v>
+      </c>
+      <c r="AX8">
+        <v>47.61</v>
+      </c>
     </row>
-    <row r="9" spans="1:48">
+    <row r="9" spans="1:50">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2385,8 +2436,14 @@
       <c r="AV9">
         <v>825</v>
       </c>
+      <c r="AW9">
+        <v>353.42</v>
+      </c>
+      <c r="AX9">
+        <v>26.39</v>
+      </c>
     </row>
-    <row r="10" spans="1:48">
+    <row r="10" spans="1:50">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2531,8 +2588,14 @@
       <c r="AV10">
         <v>800</v>
       </c>
+      <c r="AW10">
+        <v>302.56</v>
+      </c>
+      <c r="AX10">
+        <v>34.159999999999997</v>
+      </c>
     </row>
-    <row r="11" spans="1:48">
+    <row r="11" spans="1:50">
       <c r="A11">
         <v>11</v>
       </c>
@@ -2677,8 +2740,14 @@
       <c r="AV11">
         <v>1000</v>
       </c>
+      <c r="AW11">
+        <v>601.9</v>
+      </c>
+      <c r="AX11">
+        <v>64.209999999999994</v>
+      </c>
     </row>
-    <row r="12" spans="1:48">
+    <row r="12" spans="1:50">
       <c r="A12">
         <v>12</v>
       </c>
@@ -2800,7 +2869,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:48">
+    <row r="13" spans="1:50">
       <c r="A13">
         <v>13</v>
       </c>
@@ -2945,8 +3014,14 @@
       <c r="AV13">
         <v>600</v>
       </c>
+      <c r="AW13">
+        <v>636.91999999999996</v>
+      </c>
+      <c r="AX13">
+        <v>67.099999999999994</v>
+      </c>
     </row>
-    <row r="14" spans="1:48">
+    <row r="14" spans="1:50">
       <c r="A14">
         <v>14</v>
       </c>
@@ -3091,8 +3166,14 @@
       <c r="AV14">
         <v>719</v>
       </c>
+      <c r="AW14">
+        <v>499.97</v>
+      </c>
+      <c r="AX14">
+        <v>69.64</v>
+      </c>
     </row>
-    <row r="15" spans="1:48">
+    <row r="15" spans="1:50">
       <c r="A15">
         <v>15</v>
       </c>
@@ -3237,8 +3318,14 @@
       <c r="AV15">
         <v>1000</v>
       </c>
+      <c r="AW15">
+        <v>378.57</v>
+      </c>
+      <c r="AX15">
+        <v>77.47</v>
+      </c>
     </row>
-    <row r="16" spans="1:48">
+    <row r="16" spans="1:50">
       <c r="A16">
         <v>16</v>
       </c>
@@ -3383,8 +3470,14 @@
       <c r="AV16">
         <v>300</v>
       </c>
+      <c r="AW16">
+        <v>281.66000000000003</v>
+      </c>
+      <c r="AX16">
+        <v>20.45</v>
+      </c>
     </row>
-    <row r="17" spans="1:48">
+    <row r="17" spans="1:50">
       <c r="A17">
         <v>17</v>
       </c>
@@ -3529,8 +3622,14 @@
       <c r="AV17">
         <v>100</v>
       </c>
+      <c r="AW17">
+        <v>519.54</v>
+      </c>
+      <c r="AX17">
+        <v>52.59</v>
+      </c>
     </row>
-    <row r="18" spans="1:48">
+    <row r="18" spans="1:50">
       <c r="A18">
         <v>18</v>
       </c>
@@ -3675,8 +3774,14 @@
       <c r="AV18">
         <v>500</v>
       </c>
+      <c r="AW18">
+        <v>423.17</v>
+      </c>
+      <c r="AX18">
+        <v>22.27</v>
+      </c>
     </row>
-    <row r="19" spans="1:48">
+    <row r="19" spans="1:50">
       <c r="A19">
         <v>19</v>
       </c>
@@ -3798,7 +3903,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:48">
+    <row r="20" spans="1:50">
       <c r="A20">
         <v>20</v>
       </c>
@@ -3920,7 +4025,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:48">
+    <row r="21" spans="1:50">
       <c r="A21">
         <v>21</v>
       </c>
@@ -4064,6 +4169,12 @@
       </c>
       <c r="AV21">
         <v>300</v>
+      </c>
+      <c r="AW21">
+        <v>580.12</v>
+      </c>
+      <c r="AX21">
+        <v>30.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrote more; added script for range size information
</commit_message>
<xml_diff>
--- a/Sheets/datasetOverview.xlsx
+++ b/Sheets/datasetOverview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="0" windowWidth="10640" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="200">
   <si>
     <t>ID</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>mnRng</t>
+  </si>
+  <si>
+    <t>pr1el</t>
   </si>
 </sst>
 </file>
@@ -1088,13 +1091,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX21"/>
+  <dimension ref="A1:AY21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AX21" sqref="AX21"/>
+      <selection pane="bottomRight" activeCell="AY22" sqref="AY22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1105,7 +1108,7 @@
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:51">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1256,8 +1259,11 @@
       <c r="AX1" t="s">
         <v>197</v>
       </c>
+      <c r="AY1" t="s">
+        <v>199</v>
+      </c>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:51">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1408,8 +1414,11 @@
       <c r="AX2">
         <v>57.04</v>
       </c>
+      <c r="AY2">
+        <v>0.20133999999999999</v>
+      </c>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:51">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1560,8 +1569,11 @@
       <c r="AX3">
         <v>64</v>
       </c>
+      <c r="AY3">
+        <v>0.18182000000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:51">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1712,8 +1724,11 @@
       <c r="AX4">
         <v>52.04</v>
       </c>
+      <c r="AY4">
+        <v>0.25502999999999998</v>
+      </c>
     </row>
-    <row r="5" spans="1:50">
+    <row r="5" spans="1:51">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1864,8 +1879,11 @@
       <c r="AX5">
         <v>34.83</v>
       </c>
+      <c r="AY5">
+        <v>0.25925999999999999</v>
+      </c>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:51">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2016,8 +2034,11 @@
       <c r="AX6">
         <v>50.75</v>
       </c>
+      <c r="AY6">
+        <v>0.12739</v>
+      </c>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:51">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2139,7 +2160,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:50">
+    <row r="8" spans="1:51">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2290,8 +2311,11 @@
       <c r="AX8">
         <v>47.61</v>
       </c>
+      <c r="AY8">
+        <v>0.55769000000000002</v>
+      </c>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:51">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2442,8 +2466,11 @@
       <c r="AX9">
         <v>26.39</v>
       </c>
+      <c r="AY9">
+        <v>0.44374999999999998</v>
+      </c>
     </row>
-    <row r="10" spans="1:50">
+    <row r="10" spans="1:51">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2594,8 +2621,11 @@
       <c r="AX10">
         <v>34.159999999999997</v>
       </c>
+      <c r="AY10">
+        <v>0.10256</v>
+      </c>
     </row>
-    <row r="11" spans="1:50">
+    <row r="11" spans="1:51">
       <c r="A11">
         <v>11</v>
       </c>
@@ -2746,8 +2776,11 @@
       <c r="AX11">
         <v>64.209999999999994</v>
       </c>
+      <c r="AY11">
+        <v>0.24285999999999999</v>
+      </c>
     </row>
-    <row r="12" spans="1:50">
+    <row r="12" spans="1:51">
       <c r="A12">
         <v>12</v>
       </c>
@@ -2869,7 +2902,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:50">
+    <row r="13" spans="1:51">
       <c r="A13">
         <v>13</v>
       </c>
@@ -3020,8 +3053,11 @@
       <c r="AX13">
         <v>67.099999999999994</v>
       </c>
+      <c r="AY13">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="14" spans="1:50">
+    <row r="14" spans="1:51">
       <c r="A14">
         <v>14</v>
       </c>
@@ -3172,8 +3208,11 @@
       <c r="AX14">
         <v>69.64</v>
       </c>
+      <c r="AY14">
+        <v>0.12820999999999999</v>
+      </c>
     </row>
-    <row r="15" spans="1:50">
+    <row r="15" spans="1:51">
       <c r="A15">
         <v>15</v>
       </c>
@@ -3324,8 +3363,11 @@
       <c r="AX15">
         <v>77.47</v>
       </c>
+      <c r="AY15">
+        <v>0.39285999999999999</v>
+      </c>
     </row>
-    <row r="16" spans="1:50">
+    <row r="16" spans="1:51">
       <c r="A16">
         <v>16</v>
       </c>
@@ -3476,8 +3518,11 @@
       <c r="AX16">
         <v>20.45</v>
       </c>
+      <c r="AY16">
+        <v>0.35503000000000001</v>
+      </c>
     </row>
-    <row r="17" spans="1:50">
+    <row r="17" spans="1:51">
       <c r="A17">
         <v>17</v>
       </c>
@@ -3628,8 +3673,11 @@
       <c r="AX17">
         <v>52.59</v>
       </c>
+      <c r="AY17">
+        <v>0.32184000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:50">
+    <row r="18" spans="1:51">
       <c r="A18">
         <v>18</v>
       </c>
@@ -3780,8 +3828,11 @@
       <c r="AX18">
         <v>22.27</v>
       </c>
+      <c r="AY18">
+        <v>0.31172</v>
+      </c>
     </row>
-    <row r="19" spans="1:50">
+    <row r="19" spans="1:51">
       <c r="A19">
         <v>19</v>
       </c>
@@ -3903,7 +3954,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:50">
+    <row r="20" spans="1:51">
       <c r="A20">
         <v>20</v>
       </c>
@@ -4025,7 +4076,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:50">
+    <row r="21" spans="1:51">
       <c r="A21">
         <v>21</v>
       </c>
@@ -4175,6 +4226,9 @@
       </c>
       <c r="AX21">
         <v>30.31</v>
+      </c>
+      <c r="AY21">
+        <v>0.16667000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added rapoport's rule code; support is not high.
</commit_message>
<xml_diff>
--- a/Sheets/datasetOverview.xlsx
+++ b/Sheets/datasetOverview.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="209">
   <si>
     <t>ID</t>
   </si>
@@ -619,6 +619,33 @@
   </si>
   <si>
     <t>pr1el</t>
+  </si>
+  <si>
+    <t>stevens.p</t>
+  </si>
+  <si>
+    <t>stevens.b</t>
+  </si>
+  <si>
+    <t>stevens.r</t>
+  </si>
+  <si>
+    <t>mp.b</t>
+  </si>
+  <si>
+    <t>mp.p</t>
+  </si>
+  <si>
+    <t>mp.r</t>
+  </si>
+  <si>
+    <t>quart.b</t>
+  </si>
+  <si>
+    <t>quart.p</t>
+  </si>
+  <si>
+    <t>quart.r</t>
   </si>
 </sst>
 </file>
@@ -714,8 +741,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1091,13 +1119,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY21"/>
+  <dimension ref="A1:BH21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY22" sqref="AY22"/>
+      <selection pane="bottomRight" activeCell="AZ8" sqref="AZ8:BH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1108,7 +1136,7 @@
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:60">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1262,8 +1290,35 @@
       <c r="AY1" t="s">
         <v>199</v>
       </c>
+      <c r="AZ1" t="s">
+        <v>201</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>200</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>202</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>204</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>205</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>206</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>207</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>208</v>
+      </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:60">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1417,8 +1472,35 @@
       <c r="AY2">
         <v>0.20133999999999999</v>
       </c>
+      <c r="AZ2">
+        <v>0.41586990734776402</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>2.5698035198336401E-17</v>
+      </c>
+      <c r="BB2">
+        <v>0.90383766495637996</v>
+      </c>
+      <c r="BC2">
+        <v>1.0426166602909499</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>2.9849006417724198E-8</v>
+      </c>
+      <c r="BE2">
+        <v>0.84314601571570402</v>
+      </c>
+      <c r="BF2">
+        <v>0.13754863532348699</v>
+      </c>
+      <c r="BG2">
+        <v>2.36044354496672E-3</v>
+      </c>
+      <c r="BH2">
+        <v>0.42839452582674498</v>
+      </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:60">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1572,8 +1654,35 @@
       <c r="AY3">
         <v>0.18182000000000001</v>
       </c>
+      <c r="AZ3">
+        <v>0.348858294580916</v>
+      </c>
+      <c r="BA3" s="1">
+        <v>5.28512838818042E-14</v>
+      </c>
+      <c r="BB3">
+        <v>0.89055601035973098</v>
+      </c>
+      <c r="BC3">
+        <v>0.11514084927944</v>
+      </c>
+      <c r="BD3">
+        <v>0.61311412481751904</v>
+      </c>
+      <c r="BE3">
+        <v>1.5367838413272E-2</v>
+      </c>
+      <c r="BF3">
+        <v>-0.14013646754939699</v>
+      </c>
+      <c r="BG3">
+        <v>4.1492974391440098E-2</v>
+      </c>
+      <c r="BH3">
+        <v>0.21119970276444999</v>
+      </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:60">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1727,8 +1836,35 @@
       <c r="AY4">
         <v>0.25502999999999998</v>
       </c>
+      <c r="AZ4">
+        <v>-4.6263718581239503E-2</v>
+      </c>
+      <c r="BA4">
+        <v>0.40032297457278399</v>
+      </c>
+      <c r="BB4">
+        <v>3.2354327225980202E-2</v>
+      </c>
+      <c r="BC4">
+        <v>-1.15092535149761E-2</v>
+      </c>
+      <c r="BD4">
+        <v>0.92905965520506295</v>
+      </c>
+      <c r="BE4">
+        <v>4.0624451879094097E-4</v>
+      </c>
+      <c r="BF4">
+        <v>-1.10955230787968E-2</v>
+      </c>
+      <c r="BG4">
+        <v>0.76368122778972802</v>
+      </c>
+      <c r="BH4">
+        <v>4.1942221872483297E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:60">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1882,8 +2018,35 @@
       <c r="AY5">
         <v>0.25925999999999999</v>
       </c>
+      <c r="AZ5">
+        <v>3.5787540253144302E-3</v>
+      </c>
+      <c r="BA5">
+        <v>0.94250203263674504</v>
+      </c>
+      <c r="BB5">
+        <v>4.5182725419334597E-4</v>
+      </c>
+      <c r="BC5">
+        <v>0.14741465456706099</v>
+      </c>
+      <c r="BD5">
+        <v>0.342454839628338</v>
+      </c>
+      <c r="BE5">
+        <v>0.100386206182037</v>
+      </c>
+      <c r="BF5">
+        <v>-8.3140289662030006E-3</v>
+      </c>
+      <c r="BG5">
+        <v>0.80407182602178096</v>
+      </c>
+      <c r="BH5">
+        <v>6.4483601830224602E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:60">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2037,8 +2200,35 @@
       <c r="AY6">
         <v>0.12739</v>
       </c>
+      <c r="AZ6">
+        <v>0.19484612780494501</v>
+      </c>
+      <c r="BA6" s="1">
+        <v>4.25726378656153E-11</v>
+      </c>
+      <c r="BB6">
+        <v>0.71595356615356198</v>
+      </c>
+      <c r="BC6">
+        <v>0.17533689866086499</v>
+      </c>
+      <c r="BD6">
+        <v>5.4672859670186702E-2</v>
+      </c>
+      <c r="BE6">
+        <v>0.15125821648877699</v>
+      </c>
+      <c r="BF6">
+        <v>-2.0336641438585799E-2</v>
+      </c>
+      <c r="BG6">
+        <v>0.31974550962197701</v>
+      </c>
+      <c r="BH6">
+        <v>3.2995840210415101E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:60">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2160,7 +2350,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:60">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2314,8 +2504,35 @@
       <c r="AY8">
         <v>0.55769000000000002</v>
       </c>
+      <c r="AZ8">
+        <v>-1.9190487083708501E-2</v>
+      </c>
+      <c r="BA8">
+        <v>0.87111480497997895</v>
+      </c>
+      <c r="BB8">
+        <v>5.7973238301720796E-3</v>
+      </c>
+      <c r="BC8">
+        <v>-6.2734561583077303E-2</v>
+      </c>
+      <c r="BD8">
+        <v>0.81931404070529001</v>
+      </c>
+      <c r="BE8">
+        <v>6.1092686968426202E-3</v>
+      </c>
+      <c r="BF8">
+        <v>7.7205882352941194E-2</v>
+      </c>
+      <c r="BG8">
+        <v>0.28155001721318301</v>
+      </c>
+      <c r="BH8">
+        <v>8.2235461945120394E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:60">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2469,8 +2686,35 @@
       <c r="AY9">
         <v>0.44374999999999998</v>
       </c>
+      <c r="AZ9">
+        <v>-0.15621454096475801</v>
+      </c>
+      <c r="BA9">
+        <v>2.8987107126795E-2</v>
+      </c>
+      <c r="BB9">
+        <v>0.64784058836479097</v>
+      </c>
+      <c r="BC9">
+        <v>-0.15484096571993999</v>
+      </c>
+      <c r="BD9">
+        <v>0.27979585944087798</v>
+      </c>
+      <c r="BE9">
+        <v>9.6464301932903895E-2</v>
+      </c>
+      <c r="BF9">
+        <v>-2.15798825020657E-2</v>
+      </c>
+      <c r="BG9">
+        <v>0.50998841948861395</v>
+      </c>
+      <c r="BH9">
+        <v>2.3181660699621399E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:51">
+    <row r="10" spans="1:60">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2624,8 +2868,35 @@
       <c r="AY10">
         <v>0.10256</v>
       </c>
+      <c r="AZ10">
+        <v>0.183967229931564</v>
+      </c>
+      <c r="BA10">
+        <v>2.99664279597286E-3</v>
+      </c>
+      <c r="BB10">
+        <v>0.79347979439445404</v>
+      </c>
+      <c r="BC10">
+        <v>3.4506556245655299E-4</v>
+      </c>
+      <c r="BD10">
+        <v>0.99924644725830503</v>
+      </c>
+      <c r="BE10" s="1">
+        <v>2.5237414669102799E-7</v>
+      </c>
+      <c r="BF10">
+        <v>5.6141774891775E-2</v>
+      </c>
+      <c r="BG10">
+        <v>0.33323170902379201</v>
+      </c>
+      <c r="BH10">
+        <v>0.15577360990063599</v>
+      </c>
     </row>
-    <row r="11" spans="1:51">
+    <row r="11" spans="1:60">
       <c r="A11">
         <v>11</v>
       </c>
@@ -2779,8 +3050,35 @@
       <c r="AY11">
         <v>0.24285999999999999</v>
       </c>
+      <c r="AZ11">
+        <v>4.9118965362585101E-2</v>
+      </c>
+      <c r="BA11">
+        <v>0.41544744799825201</v>
+      </c>
+      <c r="BB11">
+        <v>3.03638340828889E-2</v>
+      </c>
+      <c r="BC11">
+        <v>0.30317226890756299</v>
+      </c>
+      <c r="BD11">
+        <v>0.216680125273289</v>
+      </c>
+      <c r="BE11">
+        <v>0.10679317127647001</v>
+      </c>
+      <c r="BF11">
+        <v>0.13804794138770299</v>
+      </c>
+      <c r="BG11">
+        <v>6.4349045259537102E-3</v>
+      </c>
+      <c r="BH11">
+        <v>0.30357003453746401</v>
+      </c>
     </row>
-    <row r="12" spans="1:51">
+    <row r="12" spans="1:60">
       <c r="A12">
         <v>12</v>
       </c>
@@ -2902,7 +3200,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:51">
+    <row r="13" spans="1:60">
       <c r="A13">
         <v>13</v>
       </c>
@@ -3056,8 +3354,35 @@
       <c r="AY13">
         <v>0.2</v>
       </c>
+      <c r="AZ13">
+        <v>0.38095009808832198</v>
+      </c>
+      <c r="BA13" s="1">
+        <v>1.5288364579422501E-9</v>
+      </c>
+      <c r="BB13">
+        <v>0.90362274121711805</v>
+      </c>
+      <c r="BC13">
+        <v>0.541219256933543</v>
+      </c>
+      <c r="BD13">
+        <v>7.0596492103952996E-2</v>
+      </c>
+      <c r="BE13">
+        <v>0.24701663211101199</v>
+      </c>
+      <c r="BF13">
+        <v>0.120952394249891</v>
+      </c>
+      <c r="BG13">
+        <v>1.62230060488644E-2</v>
+      </c>
+      <c r="BH13">
+        <v>0.34765903493539002</v>
+      </c>
     </row>
-    <row r="14" spans="1:51">
+    <row r="14" spans="1:60">
       <c r="A14">
         <v>14</v>
       </c>
@@ -3211,8 +3536,35 @@
       <c r="AY14">
         <v>0.12820999999999999</v>
       </c>
+      <c r="AZ14">
+        <v>0.53694481569770802</v>
+      </c>
+      <c r="BA14" s="1">
+        <v>1.02133222199013E-11</v>
+      </c>
+      <c r="BB14">
+        <v>0.91691758045595595</v>
+      </c>
+      <c r="BC14">
+        <v>1.6233784013605399</v>
+      </c>
+      <c r="BD14">
+        <v>3.8245045735103302E-3</v>
+      </c>
+      <c r="BE14">
+        <v>0.77656202841275301</v>
+      </c>
+      <c r="BF14">
+        <v>-0.36661904761904801</v>
+      </c>
+      <c r="BG14">
+        <v>9.1002277989133198E-2</v>
+      </c>
+      <c r="BH14">
+        <v>0.55113015542960597</v>
+      </c>
     </row>
-    <row r="15" spans="1:51">
+    <row r="15" spans="1:60">
       <c r="A15">
         <v>15</v>
       </c>
@@ -3366,8 +3718,35 @@
       <c r="AY15">
         <v>0.39285999999999999</v>
       </c>
+      <c r="AZ15">
+        <v>9.2904811580424004E-2</v>
+      </c>
+      <c r="BA15">
+        <v>0.65544510303558001</v>
+      </c>
+      <c r="BB15">
+        <v>7.51221266857868E-2</v>
+      </c>
+      <c r="BC15">
+        <v>-3.6590909090909E-2</v>
+      </c>
+      <c r="BD15">
+        <v>0.91599820807399102</v>
+      </c>
+      <c r="BE15">
+        <v>1.70510459150112E-3</v>
+      </c>
+      <c r="BF15">
+        <v>-0.331060606060606</v>
+      </c>
+      <c r="BG15">
+        <v>1.14388979396833E-2</v>
+      </c>
+      <c r="BH15">
+        <v>0.62287665692516403</v>
+      </c>
     </row>
-    <row r="16" spans="1:51">
+    <row r="16" spans="1:60">
       <c r="A16">
         <v>16</v>
       </c>
@@ -3521,8 +3900,35 @@
       <c r="AY16">
         <v>0.35503000000000001</v>
       </c>
+      <c r="AZ16">
+        <v>0.31583780485594698</v>
+      </c>
+      <c r="BA16">
+        <v>3.0752312035444399E-3</v>
+      </c>
+      <c r="BB16">
+        <v>0.962836435815698</v>
+      </c>
+      <c r="BC16">
+        <v>-0.105555555555556</v>
+      </c>
+      <c r="BD16">
+        <v>0.72721198827390299</v>
+      </c>
+      <c r="BE16">
+        <v>1.8491242824647699E-2</v>
+      </c>
+      <c r="BF16">
+        <v>5.8412698412698402E-2</v>
+      </c>
+      <c r="BG16">
+        <v>0.364487902659763</v>
+      </c>
+      <c r="BH16">
+        <v>0.118428941662146</v>
+      </c>
     </row>
-    <row r="17" spans="1:51">
+    <row r="17" spans="1:60">
       <c r="A17">
         <v>17</v>
       </c>
@@ -3676,8 +4082,35 @@
       <c r="AY17">
         <v>0.32184000000000001</v>
       </c>
+      <c r="AZ17">
+        <v>-3.9664473705920002E-2</v>
+      </c>
+      <c r="BA17">
+        <v>0.72447486705119601</v>
+      </c>
+      <c r="BB17">
+        <v>7.9794943386260007E-3</v>
+      </c>
+      <c r="BC17">
+        <v>-0.17567232385142101</v>
+      </c>
+      <c r="BD17">
+        <v>0.45467693864973902</v>
+      </c>
+      <c r="BE17">
+        <v>4.7391795199514399E-2</v>
+      </c>
+      <c r="BF17">
+        <v>-4.01511000916226E-2</v>
+      </c>
+      <c r="BG17">
+        <v>0.46970647693905199</v>
+      </c>
+      <c r="BH17">
+        <v>3.5379848534768402E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:51">
+    <row r="18" spans="1:60">
       <c r="A18">
         <v>18</v>
       </c>
@@ -3831,8 +4264,35 @@
       <c r="AY18">
         <v>0.31172</v>
       </c>
+      <c r="AZ18">
+        <v>0.19753394019575199</v>
+      </c>
+      <c r="BA18">
+        <v>1.46400859244754E-3</v>
+      </c>
+      <c r="BB18">
+        <v>0.88866651107341799</v>
+      </c>
+      <c r="BC18">
+        <v>5.8672253295815803E-2</v>
+      </c>
+      <c r="BD18">
+        <v>0.81054514593314297</v>
+      </c>
+      <c r="BE18">
+        <v>4.2448177063020998E-3</v>
+      </c>
+      <c r="BF18">
+        <v>-1.0726099661540599E-2</v>
+      </c>
+      <c r="BG18">
+        <v>0.82330755457079596</v>
+      </c>
+      <c r="BH18">
+        <v>2.6904953189824101E-3</v>
+      </c>
     </row>
-    <row r="19" spans="1:51">
+    <row r="19" spans="1:60">
       <c r="A19">
         <v>19</v>
       </c>
@@ -3954,7 +4414,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:51">
+    <row r="20" spans="1:60">
       <c r="A20">
         <v>20</v>
       </c>
@@ -4076,7 +4536,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:51">
+    <row r="21" spans="1:60">
       <c r="A21">
         <v>21</v>
       </c>
@@ -4229,6 +4689,33 @@
       </c>
       <c r="AY21">
         <v>0.16667000000000001</v>
+      </c>
+      <c r="AZ21">
+        <v>0.14581039625564801</v>
+      </c>
+      <c r="BA21">
+        <v>1.39586132450954E-2</v>
+      </c>
+      <c r="BB21">
+        <v>0.40787072319447598</v>
+      </c>
+      <c r="BC21">
+        <v>0.13276075050709901</v>
+      </c>
+      <c r="BD21">
+        <v>0.66285647954021498</v>
+      </c>
+      <c r="BE21">
+        <v>2.2073426996247699E-2</v>
+      </c>
+      <c r="BF21">
+        <v>-7.9386294765840207E-2</v>
+      </c>
+      <c r="BG21">
+        <v>7.2252958943289702E-2</v>
+      </c>
+      <c r="BH21">
+        <v>0.31530394276905899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added multisite beta indices; wrote some; ideas from meeting with Christy
</commit_message>
<xml_diff>
--- a/Sheets/datasetOverview.xlsx
+++ b/Sheets/datasetOverview.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="218">
   <si>
     <t>ID</t>
   </si>
@@ -646,6 +646,33 @@
   </si>
   <si>
     <t>quart.r</t>
+  </si>
+  <si>
+    <t>sp.sim</t>
+  </si>
+  <si>
+    <t>sp.sne</t>
+  </si>
+  <si>
+    <t>sp.sor</t>
+  </si>
+  <si>
+    <t>gen.sim</t>
+  </si>
+  <si>
+    <t>gen.sne</t>
+  </si>
+  <si>
+    <t>gen.sor</t>
+  </si>
+  <si>
+    <t>sf.sim</t>
+  </si>
+  <si>
+    <t>sf.sne</t>
+  </si>
+  <si>
+    <t>sf.sor</t>
   </si>
 </sst>
 </file>
@@ -694,8 +721,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -745,7 +774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -768,6 +797,7 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -790,6 +820,7 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1119,13 +1150,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BH21"/>
+  <dimension ref="A1:BQ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="BC2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ8" sqref="AZ8:BH11"/>
+      <selection pane="bottomRight" activeCell="BI8" sqref="BI8:BQ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1136,7 +1167,7 @@
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60">
+    <row r="1" spans="1:69">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1317,8 +1348,35 @@
       <c r="BH1" t="s">
         <v>208</v>
       </c>
+      <c r="BI1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>210</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>211</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>212</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>213</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>215</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>216</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>217</v>
+      </c>
     </row>
-    <row r="2" spans="1:60">
+    <row r="2" spans="1:69">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1499,8 +1557,35 @@
       <c r="BH2">
         <v>0.42839452582674498</v>
       </c>
+      <c r="BI2">
+        <v>0.63912164114417802</v>
+      </c>
+      <c r="BJ2">
+        <v>0.26650024188438498</v>
+      </c>
+      <c r="BK2">
+        <v>0.90562188302856295</v>
+      </c>
+      <c r="BL2">
+        <v>0.38286713286713298</v>
+      </c>
+      <c r="BM2">
+        <v>0.50384660269127501</v>
+      </c>
+      <c r="BN2">
+        <v>0.88671373555840804</v>
+      </c>
+      <c r="BO2">
+        <v>4.1237113402061903E-2</v>
+      </c>
+      <c r="BP2">
+        <v>0.76818911610613505</v>
+      </c>
+      <c r="BQ2">
+        <v>0.80942622950819698</v>
+      </c>
     </row>
-    <row r="3" spans="1:60">
+    <row r="3" spans="1:69">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1681,8 +1766,35 @@
       <c r="BH3">
         <v>0.21119970276444999</v>
       </c>
+      <c r="BI3">
+        <v>0.62353775257001098</v>
+      </c>
+      <c r="BJ3">
+        <v>0.24633113604658</v>
+      </c>
+      <c r="BK3">
+        <v>0.86986888861659095</v>
+      </c>
+      <c r="BL3">
+        <v>0.47217806041335503</v>
+      </c>
+      <c r="BM3">
+        <v>0.355085207016406</v>
+      </c>
+      <c r="BN3">
+        <v>0.82726326742976097</v>
+      </c>
+      <c r="BO3">
+        <v>0</v>
+      </c>
+      <c r="BP3">
+        <v>0.693965517241379</v>
+      </c>
+      <c r="BQ3">
+        <v>0.693965517241379</v>
+      </c>
     </row>
-    <row r="4" spans="1:60">
+    <row r="4" spans="1:69">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1863,8 +1975,35 @@
       <c r="BH4">
         <v>4.1942221872483297E-3</v>
       </c>
+      <c r="BI4">
+        <v>0.62104514752932805</v>
+      </c>
+      <c r="BJ4">
+        <v>0.23929809890064699</v>
+      </c>
+      <c r="BK4">
+        <v>0.86034324642997495</v>
+      </c>
+      <c r="BL4">
+        <v>0.493365500603136</v>
+      </c>
+      <c r="BM4">
+        <v>0.28423577024674501</v>
+      </c>
+      <c r="BN4">
+        <v>0.77760127084988095</v>
+      </c>
+      <c r="BO4">
+        <v>2.8846153846153799E-2</v>
+      </c>
+      <c r="BP4">
+        <v>0.60979427549194998</v>
+      </c>
+      <c r="BQ4">
+        <v>0.63864042933810405</v>
+      </c>
     </row>
-    <row r="5" spans="1:60">
+    <row r="5" spans="1:69">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2045,8 +2184,35 @@
       <c r="BH5">
         <v>6.4483601830224602E-3</v>
       </c>
+      <c r="BI5">
+        <v>0.63092269326683303</v>
+      </c>
+      <c r="BJ5">
+        <v>0.19124612619847201</v>
+      </c>
+      <c r="BK5">
+        <v>0.82216881946530496</v>
+      </c>
+      <c r="BL5">
+        <v>0.38768115942029002</v>
+      </c>
+      <c r="BM5">
+        <v>0.35070893345896698</v>
+      </c>
+      <c r="BN5">
+        <v>0.73839009287925705</v>
+      </c>
+      <c r="BO5">
+        <v>0.06</v>
+      </c>
+      <c r="BP5">
+        <v>0.60784452296819802</v>
+      </c>
+      <c r="BQ5">
+        <v>0.66784452296819796</v>
+      </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:69">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2227,8 +2393,35 @@
       <c r="BH6">
         <v>3.2995840210415101E-2</v>
       </c>
+      <c r="BI6">
+        <v>0.82718204488778102</v>
+      </c>
+      <c r="BJ6">
+        <v>9.6820696716057697E-2</v>
+      </c>
+      <c r="BK6">
+        <v>0.924002741603838</v>
+      </c>
+      <c r="BL6">
+        <v>0.66917859834212501</v>
+      </c>
+      <c r="BM6">
+        <v>0.21747257645777199</v>
+      </c>
+      <c r="BN6">
+        <v>0.88665117479989697</v>
+      </c>
+      <c r="BO6">
+        <v>2.04081632653061E-2</v>
+      </c>
+      <c r="BP6">
+        <v>0.57538131041890395</v>
+      </c>
+      <c r="BQ6">
+        <v>0.59578947368421098</v>
+      </c>
     </row>
-    <row r="7" spans="1:60">
+    <row r="7" spans="1:69">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2350,7 +2543,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:60">
+    <row r="8" spans="1:69">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2531,8 +2724,35 @@
       <c r="BH8">
         <v>8.2235461945120394E-2</v>
       </c>
+      <c r="BI8">
+        <v>0.65354330708661401</v>
+      </c>
+      <c r="BJ8">
+        <v>0.17390767330554299</v>
+      </c>
+      <c r="BK8">
+        <v>0.82745098039215703</v>
+      </c>
+      <c r="BL8">
+        <v>0.50704225352112697</v>
+      </c>
+      <c r="BM8">
+        <v>0.219520246478873</v>
+      </c>
+      <c r="BN8">
+        <v>0.7265625</v>
+      </c>
+      <c r="BO8">
+        <v>0</v>
+      </c>
+      <c r="BP8">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="BQ8">
+        <v>0.53333333333333299</v>
+      </c>
     </row>
-    <row r="9" spans="1:60">
+    <row r="9" spans="1:69">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2713,8 +2933,35 @@
       <c r="BH9">
         <v>2.3181660699621399E-2</v>
       </c>
+      <c r="BI9">
+        <v>0.66305525460454995</v>
+      </c>
+      <c r="BJ9">
+        <v>0.11839239121414299</v>
+      </c>
+      <c r="BK9">
+        <v>0.78144764581869297</v>
+      </c>
+      <c r="BL9">
+        <v>0.125</v>
+      </c>
+      <c r="BM9">
+        <v>0.32327586206896602</v>
+      </c>
+      <c r="BN9">
+        <v>0.44827586206896602</v>
+      </c>
+      <c r="BO9">
+        <v>0</v>
+      </c>
+      <c r="BP9">
+        <v>0.29310344827586199</v>
+      </c>
+      <c r="BQ9">
+        <v>0.29310344827586199</v>
+      </c>
     </row>
-    <row r="10" spans="1:60">
+    <row r="10" spans="1:69">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2895,8 +3142,35 @@
       <c r="BH10">
         <v>0.15577360990063599</v>
       </c>
+      <c r="BI10">
+        <v>0.36216216216216202</v>
+      </c>
+      <c r="BJ10">
+        <v>0.294315275974665</v>
+      </c>
+      <c r="BK10">
+        <v>0.65647743813682702</v>
+      </c>
+      <c r="BL10">
+        <v>0.2</v>
+      </c>
+      <c r="BM10">
+        <v>0.37088122605363999</v>
+      </c>
+      <c r="BN10">
+        <v>0.57088122605364</v>
+      </c>
+      <c r="BO10">
+        <v>0</v>
+      </c>
+      <c r="BP10">
+        <v>0.44144144144144098</v>
+      </c>
+      <c r="BQ10">
+        <v>0.44144144144144098</v>
+      </c>
     </row>
-    <row r="11" spans="1:60">
+    <row r="11" spans="1:69">
       <c r="A11">
         <v>11</v>
       </c>
@@ -3077,8 +3351,35 @@
       <c r="BH11">
         <v>0.30357003453746401</v>
       </c>
+      <c r="BI11">
+        <v>0.71348314606741603</v>
+      </c>
+      <c r="BJ11">
+        <v>0.16144021383448501</v>
+      </c>
+      <c r="BK11">
+        <v>0.87492335990190095</v>
+      </c>
+      <c r="BL11">
+        <v>0.58628841607564997</v>
+      </c>
+      <c r="BM11">
+        <v>0.23940879507972801</v>
+      </c>
+      <c r="BN11">
+        <v>0.82569721115537897</v>
+      </c>
+      <c r="BO11">
+        <v>7.4074074074074098E-2</v>
+      </c>
+      <c r="BP11">
+        <v>0.57381324986958804</v>
+      </c>
+      <c r="BQ11">
+        <v>0.647887323943662</v>
+      </c>
     </row>
-    <row r="12" spans="1:60">
+    <row r="12" spans="1:69">
       <c r="A12">
         <v>12</v>
       </c>
@@ -3200,7 +3501,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:60">
+    <row r="13" spans="1:69">
       <c r="A13">
         <v>13</v>
       </c>
@@ -3381,8 +3682,35 @@
       <c r="BH13">
         <v>0.34765903493539002</v>
       </c>
+      <c r="BI13">
+        <v>0.57538461538461505</v>
+      </c>
+      <c r="BJ13">
+        <v>0.22001938758054401</v>
+      </c>
+      <c r="BK13">
+        <v>0.79540400296515901</v>
+      </c>
+      <c r="BL13">
+        <v>0.271356783919598</v>
+      </c>
+      <c r="BM13">
+        <v>0.42273604308462098</v>
+      </c>
+      <c r="BN13">
+        <v>0.69409282700421904</v>
+      </c>
+      <c r="BO13">
+        <v>0</v>
+      </c>
+      <c r="BP13">
+        <v>0.57068062827225097</v>
+      </c>
+      <c r="BQ13">
+        <v>0.57068062827225097</v>
+      </c>
     </row>
-    <row r="14" spans="1:60">
+    <row r="14" spans="1:69">
       <c r="A14">
         <v>14</v>
       </c>
@@ -3563,8 +3891,35 @@
       <c r="BH14">
         <v>0.55113015542960597</v>
       </c>
+      <c r="BI14">
+        <v>0.60634081902245696</v>
+      </c>
+      <c r="BJ14">
+        <v>0.22548762341546599</v>
+      </c>
+      <c r="BK14">
+        <v>0.83182844243792298</v>
+      </c>
+      <c r="BL14">
+        <v>0.35666666666666702</v>
+      </c>
+      <c r="BM14">
+        <v>0.43377850162866399</v>
+      </c>
+      <c r="BN14">
+        <v>0.79044516829533096</v>
+      </c>
+      <c r="BO14">
+        <v>0</v>
+      </c>
+      <c r="BP14">
+        <v>0.71317829457364301</v>
+      </c>
+      <c r="BQ14">
+        <v>0.71317829457364301</v>
+      </c>
     </row>
-    <row r="15" spans="1:60">
+    <row r="15" spans="1:69">
       <c r="A15">
         <v>15</v>
       </c>
@@ -3745,8 +4100,35 @@
       <c r="BH15">
         <v>0.62287665692516403</v>
       </c>
+      <c r="BI15">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="BJ15">
+        <v>0.32212885154061599</v>
+      </c>
+      <c r="BK15">
+        <v>0.60784313725490202</v>
+      </c>
+      <c r="BL15">
+        <v>0.108108108108108</v>
+      </c>
+      <c r="BM15">
+        <v>0.35963382737576299</v>
+      </c>
+      <c r="BN15">
+        <v>0.467741935483871</v>
+      </c>
+      <c r="BO15">
+        <v>0</v>
+      </c>
+      <c r="BP15">
+        <v>0.21052631578947401</v>
+      </c>
+      <c r="BQ15">
+        <v>0.21052631578947401</v>
+      </c>
     </row>
-    <row r="16" spans="1:60">
+    <row r="16" spans="1:69">
       <c r="A16">
         <v>16</v>
       </c>
@@ -3927,8 +4309,35 @@
       <c r="BH16">
         <v>0.118428941662146</v>
       </c>
+      <c r="BI16">
+        <v>0.38501291989664099</v>
+      </c>
+      <c r="BJ16">
+        <v>0.229249640881317</v>
+      </c>
+      <c r="BK16">
+        <v>0.61426256077795804</v>
+      </c>
+      <c r="BL16">
+        <v>0.12258064516129</v>
+      </c>
+      <c r="BM16">
+        <v>0.29372836771424599</v>
+      </c>
+      <c r="BN16">
+        <v>0.41630901287553601</v>
+      </c>
+      <c r="BO16">
+        <v>0</v>
+      </c>
+      <c r="BP16">
+        <v>9.5238095238095205E-2</v>
+      </c>
+      <c r="BQ16">
+        <v>9.5238095238095205E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:60">
+    <row r="17" spans="1:69">
       <c r="A17">
         <v>17</v>
       </c>
@@ -4109,8 +4518,35 @@
       <c r="BH17">
         <v>3.5379848534768402E-2</v>
       </c>
+      <c r="BI17">
+        <v>0.49270482603815902</v>
+      </c>
+      <c r="BJ17">
+        <v>0.333348666361302</v>
+      </c>
+      <c r="BK17">
+        <v>0.82605349239946102</v>
+      </c>
+      <c r="BL17">
+        <v>0.253676470588235</v>
+      </c>
+      <c r="BM17">
+        <v>0.52674537906022301</v>
+      </c>
+      <c r="BN17">
+        <v>0.78042184964845895</v>
+      </c>
+      <c r="BO17">
+        <v>0</v>
+      </c>
+      <c r="BP17">
+        <v>0.64261168384879697</v>
+      </c>
+      <c r="BQ17">
+        <v>0.64261168384879697</v>
+      </c>
     </row>
-    <row r="18" spans="1:60">
+    <row r="18" spans="1:69">
       <c r="A18">
         <v>18</v>
       </c>
@@ -4291,8 +4727,35 @@
       <c r="BH18">
         <v>2.6904953189824101E-3</v>
       </c>
+      <c r="BI18">
+        <v>0.45299145299145299</v>
+      </c>
+      <c r="BJ18">
+        <v>0.25320594563134702</v>
+      </c>
+      <c r="BK18">
+        <v>0.70619739862279995</v>
+      </c>
+      <c r="BL18">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="BM18">
+        <v>0.38050314465408802</v>
+      </c>
+      <c r="BN18">
+        <v>0.54716981132075504</v>
+      </c>
+      <c r="BO18">
+        <v>0</v>
+      </c>
+      <c r="BP18">
+        <v>0.36666666666666697</v>
+      </c>
+      <c r="BQ18">
+        <v>0.36666666666666697</v>
+      </c>
     </row>
-    <row r="19" spans="1:60">
+    <row r="19" spans="1:69">
       <c r="A19">
         <v>19</v>
       </c>
@@ -4414,7 +4877,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:60">
+    <row r="20" spans="1:69">
       <c r="A20">
         <v>20</v>
       </c>
@@ -4536,7 +4999,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:60">
+    <row r="21" spans="1:69">
       <c r="A21">
         <v>21</v>
       </c>
@@ -4716,6 +5179,33 @@
       </c>
       <c r="BH21">
         <v>0.31530394276905899</v>
+      </c>
+      <c r="BI21">
+        <v>0.316114109483423</v>
+      </c>
+      <c r="BJ21">
+        <v>0.41304619586008801</v>
+      </c>
+      <c r="BK21">
+        <v>0.72916030534351195</v>
+      </c>
+      <c r="BL21">
+        <v>5.7142857142857099E-2</v>
+      </c>
+      <c r="BM21">
+        <v>0.581411359724613</v>
+      </c>
+      <c r="BN21">
+        <v>0.63855421686747005</v>
+      </c>
+      <c r="BO21">
+        <v>0</v>
+      </c>
+      <c r="BP21">
+        <v>0.471014492753623</v>
+      </c>
+      <c r="BQ21">
+        <v>0.471014492753623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added standardized beta section; added plots
</commit_message>
<xml_diff>
--- a/Sheets/datasetOverview.xlsx
+++ b/Sheets/datasetOverview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="1560" yWindow="4460" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="224">
   <si>
     <t>ID</t>
   </si>
@@ -673,6 +673,24 @@
   </si>
   <si>
     <t>sf.sor</t>
+  </si>
+  <si>
+    <t>sp.Dbeta</t>
+  </si>
+  <si>
+    <t>sp.STB</t>
+  </si>
+  <si>
+    <t>gen.Dbeta</t>
+  </si>
+  <si>
+    <t>gen.STB</t>
+  </si>
+  <si>
+    <t>sf.Dbeta</t>
+  </si>
+  <si>
+    <t>sf.STB</t>
   </si>
 </sst>
 </file>
@@ -1150,13 +1168,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BQ21"/>
+  <dimension ref="A1:BW21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="BC2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="BM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BI8" sqref="BI8:BQ11"/>
+      <selection pane="bottomRight" activeCell="BT21" sqref="BT21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1167,7 +1185,7 @@
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69">
+    <row r="1" spans="1:75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1375,8 +1393,26 @@
       <c r="BQ1" t="s">
         <v>217</v>
       </c>
+      <c r="BR1" t="s">
+        <v>218</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>219</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>220</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>221</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>222</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="2" spans="1:69">
+    <row r="2" spans="1:75">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1584,8 +1620,26 @@
       <c r="BQ2">
         <v>0.80942622950819698</v>
       </c>
+      <c r="BR2">
+        <v>3.2412656558998001</v>
+      </c>
+      <c r="BS2">
+        <v>7.0039551746868794E-2</v>
+      </c>
+      <c r="BT2">
+        <v>3.2195121951219501</v>
+      </c>
+      <c r="BU2">
+        <v>6.9359756097560996E-2</v>
+      </c>
+      <c r="BV2">
+        <v>1.90384615384615</v>
+      </c>
+      <c r="BW2">
+        <v>2.8245192307692301E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:69">
+    <row r="3" spans="1:75">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1793,8 +1847,26 @@
       <c r="BQ3">
         <v>0.693965517241379</v>
       </c>
+      <c r="BR3">
+        <v>2.6468750000000001</v>
+      </c>
+      <c r="BS3">
+        <v>6.0995370370370401E-2</v>
+      </c>
+      <c r="BT3">
+        <v>1.70822281167109</v>
+      </c>
+      <c r="BU3">
+        <v>2.6230474506336601E-2</v>
+      </c>
+      <c r="BV3">
+        <v>1.75</v>
+      </c>
+      <c r="BW3">
+        <v>2.7777777777777801E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:69">
+    <row r="4" spans="1:75">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2002,8 +2074,26 @@
       <c r="BQ4">
         <v>0.63864042933810405</v>
       </c>
+      <c r="BR4">
+        <v>2.91680261011419</v>
+      </c>
+      <c r="BS4">
+        <v>8.3339243918008399E-2</v>
+      </c>
+      <c r="BT4">
+        <v>1.8300653594771199</v>
+      </c>
+      <c r="BU4">
+        <v>3.6089798238135802E-2</v>
+      </c>
+      <c r="BV4">
+        <v>1.1111111111111101</v>
+      </c>
+      <c r="BW4">
+        <v>4.8309178743961402E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:69">
+    <row r="5" spans="1:75">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2211,8 +2301,26 @@
       <c r="BQ5">
         <v>0.66784452296819796</v>
       </c>
+      <c r="BR5">
+        <v>3.0079575596816999</v>
+      </c>
+      <c r="BS5">
+        <v>0.15445827382166899</v>
+      </c>
+      <c r="BT5">
+        <v>2.0505050505050502</v>
+      </c>
+      <c r="BU5">
+        <v>8.0808080808080801E-2</v>
+      </c>
+      <c r="BV5">
+        <v>2.0363636363636402</v>
+      </c>
+      <c r="BW5">
+        <v>7.9720279720279702E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:69">
+    <row r="6" spans="1:75">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2420,8 +2528,26 @@
       <c r="BQ6">
         <v>0.59578947368421098</v>
       </c>
+      <c r="BR6">
+        <v>3.4577380952381001</v>
+      </c>
+      <c r="BS6">
+        <v>6.8270502645502606E-2</v>
+      </c>
+      <c r="BT6">
+        <v>2.1056910569105698</v>
+      </c>
+      <c r="BU6">
+        <v>3.0713640469737999E-2</v>
+      </c>
+      <c r="BV6">
+        <v>1.77884615384615</v>
+      </c>
+      <c r="BW6">
+        <v>2.1634615384615401E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:69">
+    <row r="7" spans="1:75">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2542,8 +2668,14 @@
       <c r="AN7" t="e">
         <v>#N/A</v>
       </c>
+      <c r="BR7">
+        <v>4.05167958656331</v>
+      </c>
+      <c r="BS7">
+        <v>0.43595422665190098</v>
+      </c>
     </row>
-    <row r="8" spans="1:69">
+    <row r="8" spans="1:75">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2751,8 +2883,26 @@
       <c r="BQ8">
         <v>0.53333333333333299</v>
       </c>
+      <c r="BR8">
+        <v>3.7916666666666701</v>
+      </c>
+      <c r="BS8">
+        <v>0.46527777777777801</v>
+      </c>
+      <c r="BT8">
+        <v>2.5454545454545499</v>
+      </c>
+      <c r="BU8">
+        <v>0.25757575757575801</v>
+      </c>
+      <c r="BV8">
+        <v>1.55555555555556</v>
+      </c>
+      <c r="BW8">
+        <v>9.2592592592592601E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:69">
+    <row r="9" spans="1:75">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2960,8 +3110,26 @@
       <c r="BQ9">
         <v>0.29310344827586199</v>
       </c>
+      <c r="BR9">
+        <v>3.3345008756567398</v>
+      </c>
+      <c r="BS9">
+        <v>0.38908347927612402</v>
+      </c>
+      <c r="BT9">
+        <v>1.4</v>
+      </c>
+      <c r="BU9">
+        <v>6.6666666666666693E-2</v>
+      </c>
+      <c r="BV9">
+        <v>1.1428571428571399</v>
+      </c>
+      <c r="BW9">
+        <v>2.3809523809523801E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:69">
+    <row r="10" spans="1:75">
       <c r="A10">
         <v>10</v>
       </c>
@@ -3169,8 +3337,26 @@
       <c r="BQ10">
         <v>0.44144144144144098</v>
       </c>
+      <c r="BR10">
+        <v>1.98726114649682</v>
+      </c>
+      <c r="BS10">
+        <v>0.14103730664240199</v>
+      </c>
+      <c r="BT10">
+        <v>1.6901408450704201</v>
+      </c>
+      <c r="BU10">
+        <v>9.85915492957746E-2</v>
+      </c>
+      <c r="BV10">
+        <v>1.2972972972973</v>
+      </c>
+      <c r="BW10">
+        <v>4.2471042471042497E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:69">
+    <row r="11" spans="1:75">
       <c r="A11">
         <v>11</v>
       </c>
@@ -3378,8 +3564,26 @@
       <c r="BQ11">
         <v>0.647887323943662</v>
       </c>
+      <c r="BR11">
+        <v>3.3870967741935498</v>
+      </c>
+      <c r="BS11">
+        <v>0.103786816269285</v>
+      </c>
+      <c r="BT11">
+        <v>2.7826086956521698</v>
+      </c>
+      <c r="BU11">
+        <v>7.7504725897920596E-2</v>
+      </c>
+      <c r="BV11">
+        <v>1.68421052631579</v>
+      </c>
+      <c r="BW11">
+        <v>2.9748283752860399E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:69">
+    <row r="12" spans="1:75">
       <c r="A12">
         <v>12</v>
       </c>
@@ -3500,8 +3704,14 @@
       <c r="AN12" t="e">
         <v>#N/A</v>
       </c>
+      <c r="BR12">
+        <v>3.74</v>
+      </c>
+      <c r="BS12">
+        <v>0.27400000000000002</v>
+      </c>
     </row>
-    <row r="13" spans="1:69">
+    <row r="13" spans="1:75">
       <c r="A13">
         <v>13</v>
       </c>
@@ -3709,8 +3919,26 @@
       <c r="BQ13">
         <v>0.57068062827225097</v>
       </c>
+      <c r="BR13">
+        <v>2.44258872651357</v>
+      </c>
+      <c r="BS13">
+        <v>8.4858160383151193E-2</v>
+      </c>
+      <c r="BT13">
+        <v>1.8888888888888899</v>
+      </c>
+      <c r="BU13">
+        <v>5.22875816993464E-2</v>
+      </c>
+      <c r="BV13">
+        <v>1.6</v>
+      </c>
+      <c r="BW13">
+        <v>3.5294117647058802E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:69">
+    <row r="14" spans="1:75">
       <c r="A14">
         <v>14</v>
       </c>
@@ -3918,8 +4146,26 @@
       <c r="BQ14">
         <v>0.71317829457364301</v>
       </c>
+      <c r="BR14">
+        <v>2.4937499999999999</v>
+      </c>
+      <c r="BS14">
+        <v>7.4687500000000004E-2</v>
+      </c>
+      <c r="BT14">
+        <v>1.9718309859154901</v>
+      </c>
+      <c r="BU14">
+        <v>4.8591549295774701E-2</v>
+      </c>
+      <c r="BV14">
+        <v>1.575</v>
+      </c>
+      <c r="BW14">
+        <v>2.8750000000000001E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:69">
+    <row r="15" spans="1:75">
       <c r="A15">
         <v>15</v>
       </c>
@@ -4127,8 +4373,26 @@
       <c r="BQ15">
         <v>0.21052631578947401</v>
       </c>
+      <c r="BR15">
+        <v>2.0138888888888902</v>
+      </c>
+      <c r="BS15">
+        <v>0.25347222222222199</v>
+      </c>
+      <c r="BT15">
+        <v>1.6666666666666701</v>
+      </c>
+      <c r="BU15">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="BV15">
+        <v>1.25</v>
+      </c>
+      <c r="BW15">
+        <v>6.25E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:69">
+    <row r="16" spans="1:75">
       <c r="A16">
         <v>16</v>
       </c>
@@ -4336,8 +4600,26 @@
       <c r="BQ16">
         <v>9.5238095238095205E-2</v>
       </c>
+      <c r="BR16">
+        <v>2.0761670761670801</v>
+      </c>
+      <c r="BS16">
+        <v>0.26904176904176902</v>
+      </c>
+      <c r="BT16">
+        <v>1.5</v>
+      </c>
+      <c r="BU16">
+        <v>0.125</v>
+      </c>
+      <c r="BV16">
+        <v>1.0869565217391299</v>
+      </c>
+      <c r="BW16">
+        <v>2.1739130434782601E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:69">
+    <row r="17" spans="1:75">
       <c r="A17">
         <v>17</v>
       </c>
@@ -4545,8 +4827,26 @@
       <c r="BQ17">
         <v>0.64261168384879697</v>
       </c>
+      <c r="BR17">
+        <v>2.9053803339517601</v>
+      </c>
+      <c r="BS17">
+        <v>0.11208119611481</v>
+      </c>
+      <c r="BT17">
+        <v>2.1818181818181799</v>
+      </c>
+      <c r="BU17">
+        <v>6.9518716577540093E-2</v>
+      </c>
+      <c r="BV17">
+        <v>1.57894736842105</v>
+      </c>
+      <c r="BW17">
+        <v>3.4055727554179599E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:69">
+    <row r="18" spans="1:75">
       <c r="A18">
         <v>18</v>
       </c>
@@ -4754,8 +5054,26 @@
       <c r="BQ18">
         <v>0.36666666666666697</v>
       </c>
+      <c r="BR18">
+        <v>2.4011976047904202</v>
+      </c>
+      <c r="BS18">
+        <v>0.23353293413173701</v>
+      </c>
+      <c r="BT18">
+        <v>1.5806451612903201</v>
+      </c>
+      <c r="BU18">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="BV18">
+        <v>1.2173913043478299</v>
+      </c>
+      <c r="BW18">
+        <v>3.6231884057971002E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:69">
+    <row r="19" spans="1:75">
       <c r="A19">
         <v>19</v>
       </c>
@@ -4876,8 +5194,14 @@
       <c r="AN19" t="e">
         <v>#N/A</v>
       </c>
+      <c r="BR19">
+        <v>2.28070175438596</v>
+      </c>
+      <c r="BS19">
+        <v>0.320175438596491</v>
+      </c>
     </row>
-    <row r="20" spans="1:69">
+    <row r="20" spans="1:75">
       <c r="A20">
         <v>20</v>
       </c>
@@ -4998,8 +5322,14 @@
       <c r="AN20" t="e">
         <v>#N/A</v>
       </c>
+      <c r="BR20">
+        <v>2.2413793103448301</v>
+      </c>
+      <c r="BS20">
+        <v>0.31034482758620702</v>
+      </c>
     </row>
-    <row r="21" spans="1:69">
+    <row r="21" spans="1:75">
       <c r="A21">
         <v>21</v>
       </c>
@@ -5206,6 +5536,24 @@
       </c>
       <c r="BQ21">
         <v>0.471014492753623</v>
+      </c>
+      <c r="BR21">
+        <v>2.0784982935153602</v>
+      </c>
+      <c r="BS21">
+        <v>8.2961407193489101E-2</v>
+      </c>
+      <c r="BT21">
+        <v>1.44471744471744</v>
+      </c>
+      <c r="BU21">
+        <v>3.4209034209034199E-2</v>
+      </c>
+      <c r="BV21">
+        <v>1.27272727272727</v>
+      </c>
+      <c r="BW21">
+        <v>2.0979020979021001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated outline; new code for dominant taxa; new code for comparing beta metrics
</commit_message>
<xml_diff>
--- a/Sheets/datasetOverview.xlsx
+++ b/Sheets/datasetOverview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="4460" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="880" yWindow="6980" windowWidth="25040" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="230">
   <si>
     <t>ID</t>
   </si>
@@ -691,6 +691,24 @@
   </si>
   <si>
     <t>sf.STB</t>
+  </si>
+  <si>
+    <t>genPred.b</t>
+  </si>
+  <si>
+    <t>genPred.p</t>
+  </si>
+  <si>
+    <t>genPred.r</t>
+  </si>
+  <si>
+    <t>sfPred.b</t>
+  </si>
+  <si>
+    <t>sfPred.p</t>
+  </si>
+  <si>
+    <t>sfPred.r</t>
   </si>
 </sst>
 </file>
@@ -739,8 +757,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -792,7 +814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -816,6 +838,8 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -839,6 +863,8 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1168,13 +1194,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW21"/>
+  <dimension ref="A1:CC21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="BM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BT21" sqref="BT21"/>
+      <selection pane="bottomRight" activeCell="CA8" sqref="CA8:CC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1185,7 +1211,7 @@
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75">
+    <row r="1" spans="1:81">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1411,8 +1437,26 @@
       <c r="BW1" t="s">
         <v>223</v>
       </c>
+      <c r="BX1" t="s">
+        <v>224</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>225</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>226</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>227</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>228</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="2" spans="1:75">
+    <row r="2" spans="1:81">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1638,8 +1682,26 @@
       <c r="BW2">
         <v>2.8245192307692301E-2</v>
       </c>
+      <c r="BX2">
+        <v>1.42180484884765</v>
+      </c>
+      <c r="BY2" s="1">
+        <v>3.0530944106236201E-10</v>
+      </c>
+      <c r="BZ2">
+        <v>0.72671725441706003</v>
+      </c>
+      <c r="CA2">
+        <v>0.56969203205491004</v>
+      </c>
+      <c r="CB2" s="1">
+        <v>7.8126375012844603E-12</v>
+      </c>
+      <c r="CC2">
+        <v>0.78378593313630396</v>
+      </c>
     </row>
-    <row r="3" spans="1:75">
+    <row r="3" spans="1:81">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1865,8 +1927,26 @@
       <c r="BW3">
         <v>2.7777777777777801E-2</v>
       </c>
+      <c r="BX3">
+        <v>1.67999766464269</v>
+      </c>
+      <c r="BY3" s="1">
+        <v>4.8782830443082498E-8</v>
+      </c>
+      <c r="BZ3">
+        <v>0.688023864963898</v>
+      </c>
+      <c r="CA3">
+        <v>0.56270460841098002</v>
+      </c>
+      <c r="CB3" s="1">
+        <v>1.6871068780780699E-7</v>
+      </c>
+      <c r="CC3">
+        <v>0.65732219062437203</v>
+      </c>
     </row>
-    <row r="4" spans="1:75">
+    <row r="4" spans="1:81">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2092,8 +2172,26 @@
       <c r="BW4">
         <v>4.8309178743961402E-3</v>
       </c>
+      <c r="BX4">
+        <v>3.4242376549281901</v>
+      </c>
+      <c r="BY4" s="1">
+        <v>2.2956205048368101E-11</v>
+      </c>
+      <c r="BZ4">
+        <v>0.87388566919575195</v>
+      </c>
+      <c r="CA4">
+        <v>0.85915856936117396</v>
+      </c>
+      <c r="CB4" s="1">
+        <v>3.1092422597320099E-16</v>
+      </c>
+      <c r="CC4">
+        <v>0.95431444980059499</v>
+      </c>
     </row>
-    <row r="5" spans="1:75">
+    <row r="5" spans="1:81">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2319,8 +2417,26 @@
       <c r="BW5">
         <v>7.9720279720279702E-2</v>
       </c>
+      <c r="BX5">
+        <v>3.5598264104153698</v>
+      </c>
+      <c r="BY5">
+        <v>8.6690315630296702E-4</v>
+      </c>
+      <c r="BZ5">
+        <v>0.61724010292925102</v>
+      </c>
+      <c r="CA5">
+        <v>0.72727272727272696</v>
+      </c>
+      <c r="CB5" s="1">
+        <v>1.24568362116977E-8</v>
+      </c>
+      <c r="CC5">
+        <v>0.93856867434338798</v>
+      </c>
     </row>
-    <row r="6" spans="1:75">
+    <row r="6" spans="1:81">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2546,8 +2662,26 @@
       <c r="BW6">
         <v>2.1634615384615401E-2</v>
       </c>
+      <c r="BX6">
+        <v>1.0264635669845501</v>
+      </c>
+      <c r="BY6">
+        <v>2.2367131931195498E-3</v>
+      </c>
+      <c r="BZ6">
+        <v>0.23718103167392501</v>
+      </c>
+      <c r="CA6">
+        <v>0.63600385861634001</v>
+      </c>
+      <c r="CB6" s="1">
+        <v>1.1213952338167E-7</v>
+      </c>
+      <c r="CC6">
+        <v>0.55741549299554605</v>
+      </c>
     </row>
-    <row r="7" spans="1:75">
+    <row r="7" spans="1:81">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2675,7 +2809,7 @@
         <v>0.43595422665190098</v>
       </c>
     </row>
-    <row r="8" spans="1:75">
+    <row r="8" spans="1:81">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2901,8 +3035,26 @@
       <c r="BW8">
         <v>9.2592592592592601E-2</v>
       </c>
+      <c r="BX8">
+        <v>1.8098039215686299</v>
+      </c>
+      <c r="BY8">
+        <v>9.0560883849106003E-4</v>
+      </c>
+      <c r="BZ8">
+        <v>0.90785272804774098</v>
+      </c>
+      <c r="CA8">
+        <v>0.32634730538922202</v>
+      </c>
+      <c r="CB8">
+        <v>1.17237061607847E-2</v>
+      </c>
+      <c r="CC8">
+        <v>0.75000901810836196</v>
+      </c>
     </row>
-    <row r="9" spans="1:75">
+    <row r="9" spans="1:81">
       <c r="A9">
         <v>9</v>
       </c>
@@ -3128,8 +3280,26 @@
       <c r="BW9">
         <v>2.3809523809523801E-2</v>
       </c>
+      <c r="BX9">
+        <v>4.5060747663551401</v>
+      </c>
+      <c r="BY9">
+        <v>4.8924714506062698E-4</v>
+      </c>
+      <c r="BZ9">
+        <v>0.92774957237942202</v>
+      </c>
+      <c r="CA9">
+        <v>0.731366041797471</v>
+      </c>
+      <c r="CB9">
+        <v>1.3061792091971301E-3</v>
+      </c>
+      <c r="CC9">
+        <v>0.89355089973278101</v>
+      </c>
     </row>
-    <row r="10" spans="1:75">
+    <row r="10" spans="1:81">
       <c r="A10">
         <v>10</v>
       </c>
@@ -3355,8 +3525,26 @@
       <c r="BW10">
         <v>4.2471042471042497E-2</v>
       </c>
+      <c r="BX10">
+        <v>2.6986666666666701</v>
+      </c>
+      <c r="BY10">
+        <v>4.46288915679575E-4</v>
+      </c>
+      <c r="BZ10">
+        <v>0.88901388888888899</v>
+      </c>
+      <c r="CA10">
+        <v>1.24524714828897</v>
+      </c>
+      <c r="CB10">
+        <v>2.6264011286592398E-4</v>
+      </c>
+      <c r="CC10">
+        <v>0.90676696178908001</v>
+      </c>
     </row>
-    <row r="11" spans="1:75">
+    <row r="11" spans="1:81">
       <c r="A11">
         <v>11</v>
       </c>
@@ -3582,8 +3770,26 @@
       <c r="BW11">
         <v>2.9748283752860399E-2</v>
       </c>
+      <c r="BX11">
+        <v>1.91919294332353</v>
+      </c>
+      <c r="BY11" s="1">
+        <v>6.12635654488317E-9</v>
+      </c>
+      <c r="BZ11">
+        <v>0.79127884873279097</v>
+      </c>
+      <c r="CA11">
+        <v>0.69475847893114095</v>
+      </c>
+      <c r="CB11" s="1">
+        <v>1.0215889144410801E-8</v>
+      </c>
+      <c r="CC11">
+        <v>0.78145878828194903</v>
+      </c>
     </row>
-    <row r="12" spans="1:75">
+    <row r="12" spans="1:81">
       <c r="A12">
         <v>12</v>
       </c>
@@ -3711,7 +3917,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:75">
+    <row r="13" spans="1:81">
       <c r="A13">
         <v>13</v>
       </c>
@@ -3937,8 +4143,26 @@
       <c r="BW13">
         <v>3.5294117647058802E-2</v>
       </c>
+      <c r="BX13">
+        <v>1.3627639155470299</v>
+      </c>
+      <c r="BY13">
+        <v>1.0088981711362801E-2</v>
+      </c>
+      <c r="BZ13">
+        <v>0.34710066248188298</v>
+      </c>
+      <c r="CA13">
+        <v>0.62408682947192695</v>
+      </c>
+      <c r="CB13">
+        <v>4.5588525964168798E-4</v>
+      </c>
+      <c r="CC13">
+        <v>0.54647196996907299</v>
+      </c>
     </row>
-    <row r="14" spans="1:75">
+    <row r="14" spans="1:81">
       <c r="A14">
         <v>14</v>
       </c>
@@ -4164,8 +4388,26 @@
       <c r="BW14">
         <v>2.8750000000000001E-2</v>
       </c>
+      <c r="BX14">
+        <v>-0.90547024952015398</v>
+      </c>
+      <c r="BY14">
+        <v>0.29038082540127802</v>
+      </c>
+      <c r="BZ14">
+        <v>5.8606790177832602E-2</v>
+      </c>
+      <c r="CA14">
+        <v>0.57699680511182105</v>
+      </c>
+      <c r="CB14">
+        <v>1.2077984940436499E-3</v>
+      </c>
+      <c r="CC14">
+        <v>0.43191056784966098</v>
+      </c>
     </row>
-    <row r="15" spans="1:75">
+    <row r="15" spans="1:81">
       <c r="A15">
         <v>15</v>
       </c>
@@ -4391,8 +4633,26 @@
       <c r="BW15">
         <v>6.25E-2</v>
       </c>
+      <c r="BX15">
+        <v>5.5</v>
+      </c>
+      <c r="BY15">
+        <v>0.34989675794986702</v>
+      </c>
+      <c r="BZ15">
+        <v>0.28919694072657698</v>
+      </c>
+      <c r="CA15">
+        <v>0.886075949367089</v>
+      </c>
+      <c r="CB15">
+        <v>2.4403954578600898E-2</v>
+      </c>
+      <c r="CC15">
+        <v>0.85552160628546503</v>
+      </c>
     </row>
-    <row r="16" spans="1:75">
+    <row r="16" spans="1:81">
       <c r="A16">
         <v>16</v>
       </c>
@@ -4618,8 +4878,26 @@
       <c r="BW16">
         <v>2.1739130434782601E-2</v>
       </c>
+      <c r="BX16">
+        <v>10.8</v>
+      </c>
+      <c r="BY16">
+        <v>3.5354138128080898E-4</v>
+      </c>
+      <c r="BZ16">
+        <v>0.99116247450713801</v>
+      </c>
+      <c r="CA16">
+        <v>1.3442171518489401</v>
+      </c>
+      <c r="CB16">
+        <v>6.0556555523065601E-4</v>
+      </c>
+      <c r="CC16">
+        <v>0.98735812722867999</v>
+      </c>
     </row>
-    <row r="17" spans="1:75">
+    <row r="17" spans="1:81">
       <c r="A17">
         <v>17</v>
       </c>
@@ -4845,8 +5123,26 @@
       <c r="BW17">
         <v>3.4055727554179599E-2</v>
       </c>
+      <c r="BX17">
+        <v>6.5178173719376398</v>
+      </c>
+      <c r="BY17" s="1">
+        <v>7.31222748679628E-8</v>
+      </c>
+      <c r="BZ17">
+        <v>0.84428919381537904</v>
+      </c>
+      <c r="CA17">
+        <v>1.02165184972756</v>
+      </c>
+      <c r="CB17" s="1">
+        <v>9.1608805303591698E-12</v>
+      </c>
+      <c r="CC17">
+        <v>0.949026358894282</v>
+      </c>
     </row>
-    <row r="18" spans="1:75">
+    <row r="18" spans="1:81">
       <c r="A18">
         <v>18</v>
       </c>
@@ -5072,8 +5368,26 @@
       <c r="BW18">
         <v>3.6231884057971002E-2</v>
       </c>
+      <c r="BX18">
+        <v>3.6871915897876</v>
+      </c>
+      <c r="BY18" s="1">
+        <v>1.4930419880448399E-5</v>
+      </c>
+      <c r="BZ18">
+        <v>0.981963594218212</v>
+      </c>
+      <c r="CA18">
+        <v>0.50013046456256305</v>
+      </c>
+      <c r="CB18" s="1">
+        <v>9.8969885303613802E-7</v>
+      </c>
+      <c r="CC18">
+        <v>0.99389802858021203</v>
+      </c>
     </row>
-    <row r="19" spans="1:75">
+    <row r="19" spans="1:81">
       <c r="A19">
         <v>19</v>
       </c>
@@ -5201,7 +5515,7 @@
         <v>0.320175438596491</v>
       </c>
     </row>
-    <row r="20" spans="1:75">
+    <row r="20" spans="1:81">
       <c r="A20">
         <v>20</v>
       </c>
@@ -5329,7 +5643,7 @@
         <v>0.31034482758620702</v>
       </c>
     </row>
-    <row r="21" spans="1:75">
+    <row r="21" spans="1:81">
       <c r="A21">
         <v>21</v>
       </c>
@@ -5554,6 +5868,24 @@
       </c>
       <c r="BW21">
         <v>2.0979020979021001E-2</v>
+      </c>
+      <c r="BX21">
+        <v>7.1801242236024896</v>
+      </c>
+      <c r="BY21" s="1">
+        <v>1.6324586543937001E-5</v>
+      </c>
+      <c r="BZ21">
+        <v>0.79906432524743298</v>
+      </c>
+      <c r="CA21">
+        <v>1.0115985197220001</v>
+      </c>
+      <c r="CB21" s="1">
+        <v>3.3102885414045801E-12</v>
+      </c>
+      <c r="CC21">
+        <v>0.98437077575726295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made preliminary publication figures
</commit_message>
<xml_diff>
--- a/Sheets/datasetOverview.xlsx
+++ b/Sheets/datasetOverview.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="6980" windowWidth="25040" windowHeight="15500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="236">
   <si>
     <t>ID</t>
   </si>
@@ -709,6 +709,24 @@
   </si>
   <si>
     <t>sfPred.r</t>
+  </si>
+  <si>
+    <t>sp.mnRng</t>
+  </si>
+  <si>
+    <t>gen.mnRng</t>
+  </si>
+  <si>
+    <t>sf.mnRng</t>
+  </si>
+  <si>
+    <t>sp.medRng</t>
+  </si>
+  <si>
+    <t>gen.medRng</t>
+  </si>
+  <si>
+    <t>sf.medRng</t>
   </si>
 </sst>
 </file>
@@ -1194,13 +1212,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CC21"/>
+  <dimension ref="A1:CI21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="BM2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="BV2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CA8" sqref="CA8:CC11"/>
+      <selection pane="bottomRight" activeCell="CE4" sqref="CE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1211,7 +1229,7 @@
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81">
+    <row r="1" spans="1:87">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1455,8 +1473,26 @@
       <c r="CC1" t="s">
         <v>229</v>
       </c>
+      <c r="CD1" t="s">
+        <v>230</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>231</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>232</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>233</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>234</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>235</v>
+      </c>
     </row>
-    <row r="2" spans="1:81">
+    <row r="2" spans="1:87">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1700,8 +1736,26 @@
       <c r="CC2">
         <v>0.78378593313630396</v>
       </c>
+      <c r="CD2">
+        <v>924.62818791946302</v>
+      </c>
+      <c r="CE2">
+        <v>1275.08</v>
+      </c>
+      <c r="CF2">
+        <v>1625.6</v>
+      </c>
+      <c r="CG2">
+        <v>914.4</v>
+      </c>
+      <c r="CH2">
+        <v>1295.4000000000001</v>
+      </c>
+      <c r="CI2">
+        <v>1524</v>
+      </c>
     </row>
-    <row r="3" spans="1:81">
+    <row r="3" spans="1:87">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1945,8 +1999,26 @@
       <c r="CC3">
         <v>0.65732219062437203</v>
       </c>
+      <c r="CD3">
+        <v>951.24301487603304</v>
+      </c>
+      <c r="CE3">
+        <v>1526.34563478261</v>
+      </c>
+      <c r="CF3">
+        <v>1509.0648000000001</v>
+      </c>
+      <c r="CG3">
+        <v>944.88</v>
+      </c>
+      <c r="CH3">
+        <v>1524</v>
+      </c>
+      <c r="CI3">
+        <v>1798.9295999999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:81">
+    <row r="4" spans="1:87">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2190,8 +2262,26 @@
       <c r="CC4">
         <v>0.95431444980059499</v>
       </c>
+      <c r="CD4">
+        <v>767.38255033557004</v>
+      </c>
+      <c r="CE4">
+        <v>1250.2</v>
+      </c>
+      <c r="CF4">
+        <v>1481.1428571428601</v>
+      </c>
+      <c r="CG4">
+        <v>850</v>
+      </c>
+      <c r="CH4">
+        <v>1550</v>
+      </c>
+      <c r="CI4">
+        <v>1840</v>
+      </c>
     </row>
-    <row r="5" spans="1:81">
+    <row r="5" spans="1:87">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2435,8 +2525,26 @@
       <c r="CC5">
         <v>0.93856867434338798</v>
       </c>
+      <c r="CD5">
+        <v>365.43209876543199</v>
+      </c>
+      <c r="CE5">
+        <v>582.758620689655</v>
+      </c>
+      <c r="CF5">
+        <v>587.5</v>
+      </c>
+      <c r="CG5">
+        <v>300</v>
+      </c>
+      <c r="CH5">
+        <v>700</v>
+      </c>
+      <c r="CI5">
+        <v>650</v>
+      </c>
     </row>
-    <row r="6" spans="1:81">
+    <row r="6" spans="1:87">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2680,8 +2788,26 @@
       <c r="CC6">
         <v>0.55741549299554605</v>
       </c>
+      <c r="CD6">
+        <v>972.40460587388498</v>
+      </c>
+      <c r="CE6">
+        <v>1652.42651844286</v>
+      </c>
+      <c r="CF6">
+        <v>1968.86873612</v>
+      </c>
+      <c r="CG6">
+        <v>1066.799966</v>
+      </c>
+      <c r="CH6">
+        <v>1813.5599420999999</v>
+      </c>
+      <c r="CI6">
+        <v>3115.0559007000002</v>
+      </c>
     </row>
-    <row r="7" spans="1:81">
+    <row r="7" spans="1:87">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2809,7 +2935,7 @@
         <v>0.43595422665190098</v>
       </c>
     </row>
-    <row r="8" spans="1:81">
+    <row r="8" spans="1:87">
       <c r="A8">
         <v>8</v>
       </c>
@@ -3053,8 +3179,26 @@
       <c r="CC8">
         <v>0.75000901810836196</v>
       </c>
+      <c r="CD8">
+        <v>247.11538461538501</v>
+      </c>
+      <c r="CE8">
+        <v>491.25</v>
+      </c>
+      <c r="CF8">
+        <v>925</v>
+      </c>
+      <c r="CG8">
+        <v>0</v>
+      </c>
+      <c r="CH8">
+        <v>537.5</v>
+      </c>
+      <c r="CI8">
+        <v>987.5</v>
+      </c>
     </row>
-    <row r="9" spans="1:81">
+    <row r="9" spans="1:87">
       <c r="A9">
         <v>9</v>
       </c>
@@ -3298,8 +3442,26 @@
       <c r="CC9">
         <v>0.89355089973278101</v>
       </c>
+      <c r="CD9">
+        <v>353.41603053435102</v>
+      </c>
+      <c r="CE9">
+        <v>1243.2142857142901</v>
+      </c>
+      <c r="CF9">
+        <v>1608.75</v>
+      </c>
+      <c r="CG9">
+        <v>365</v>
+      </c>
+      <c r="CH9">
+        <v>1175</v>
+      </c>
+      <c r="CI9">
+        <v>1750</v>
+      </c>
     </row>
-    <row r="10" spans="1:81">
+    <row r="10" spans="1:87">
       <c r="A10">
         <v>10</v>
       </c>
@@ -3543,8 +3705,26 @@
       <c r="CC10">
         <v>0.90676696178908001</v>
       </c>
+      <c r="CD10">
+        <v>302.564102564103</v>
+      </c>
+      <c r="CE10">
+        <v>373.33333333333297</v>
+      </c>
+      <c r="CF10">
+        <v>516.66666666666697</v>
+      </c>
+      <c r="CG10">
+        <v>300</v>
+      </c>
+      <c r="CH10">
+        <v>400</v>
+      </c>
+      <c r="CI10">
+        <v>550</v>
+      </c>
     </row>
-    <row r="11" spans="1:81">
+    <row r="11" spans="1:87">
       <c r="A11">
         <v>11</v>
       </c>
@@ -3788,8 +3968,26 @@
       <c r="CC11">
         <v>0.78145878828194903</v>
       </c>
+      <c r="CD11">
+        <v>601.9</v>
+      </c>
+      <c r="CE11">
+        <v>755.83333333333303</v>
+      </c>
+      <c r="CF11">
+        <v>1300</v>
+      </c>
+      <c r="CG11">
+        <v>500</v>
+      </c>
+      <c r="CH11">
+        <v>475</v>
+      </c>
+      <c r="CI11">
+        <v>1350</v>
+      </c>
     </row>
-    <row r="12" spans="1:81">
+    <row r="12" spans="1:87">
       <c r="A12">
         <v>12</v>
       </c>
@@ -3917,7 +4115,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:81">
+    <row r="13" spans="1:87">
       <c r="A13">
         <v>13</v>
       </c>
@@ -4161,8 +4359,26 @@
       <c r="CC13">
         <v>0.54647196996907299</v>
       </c>
+      <c r="CD13">
+        <v>636.92307692307702</v>
+      </c>
+      <c r="CE13">
+        <v>852.94117647058795</v>
+      </c>
+      <c r="CF13">
+        <v>1025</v>
+      </c>
+      <c r="CG13">
+        <v>600</v>
+      </c>
+      <c r="CH13">
+        <v>1000</v>
+      </c>
+      <c r="CI13">
+        <v>1150</v>
+      </c>
     </row>
-    <row r="14" spans="1:81">
+    <row r="14" spans="1:87">
       <c r="A14">
         <v>14</v>
       </c>
@@ -4406,8 +4622,26 @@
       <c r="CC14">
         <v>0.43191056784966098</v>
       </c>
+      <c r="CD14">
+        <v>499.97435897435901</v>
+      </c>
+      <c r="CE14">
+        <v>621.85</v>
+      </c>
+      <c r="CF14">
+        <v>791</v>
+      </c>
+      <c r="CG14">
+        <v>340</v>
+      </c>
+      <c r="CH14">
+        <v>562</v>
+      </c>
+      <c r="CI14">
+        <v>856.5</v>
+      </c>
     </row>
-    <row r="15" spans="1:81">
+    <row r="15" spans="1:87">
       <c r="A15">
         <v>15</v>
       </c>
@@ -4651,8 +4885,26 @@
       <c r="CC15">
         <v>0.85552160628546503</v>
       </c>
+      <c r="CD15">
+        <v>378.57142857142901</v>
+      </c>
+      <c r="CE15">
+        <v>541.17647058823502</v>
+      </c>
+      <c r="CF15">
+        <v>950</v>
+      </c>
+      <c r="CG15">
+        <v>300</v>
+      </c>
+      <c r="CH15">
+        <v>400</v>
+      </c>
+      <c r="CI15">
+        <v>1350</v>
+      </c>
     </row>
-    <row r="16" spans="1:81">
+    <row r="16" spans="1:87">
       <c r="A16">
         <v>16</v>
       </c>
@@ -4896,8 +5148,26 @@
       <c r="CC16">
         <v>0.98735812722867999</v>
       </c>
+      <c r="CD16">
+        <v>281.65680473372799</v>
+      </c>
+      <c r="CE16">
+        <v>477.19298245613999</v>
+      </c>
+      <c r="CF16">
+        <v>760</v>
+      </c>
+      <c r="CG16">
+        <v>200</v>
+      </c>
+      <c r="CH16">
+        <v>600</v>
+      </c>
+      <c r="CI16">
+        <v>800</v>
+      </c>
     </row>
-    <row r="17" spans="1:81">
+    <row r="17" spans="1:87">
       <c r="A17">
         <v>17</v>
       </c>
@@ -5141,8 +5411,26 @@
       <c r="CC17">
         <v>0.949026358894282</v>
       </c>
+      <c r="CD17">
+        <v>519.54022988505699</v>
+      </c>
+      <c r="CE17">
+        <v>725</v>
+      </c>
+      <c r="CF17">
+        <v>1040</v>
+      </c>
+      <c r="CG17">
+        <v>400</v>
+      </c>
+      <c r="CH17">
+        <v>800</v>
+      </c>
+      <c r="CI17">
+        <v>1100</v>
+      </c>
     </row>
-    <row r="18" spans="1:81">
+    <row r="18" spans="1:87">
       <c r="A18">
         <v>18</v>
       </c>
@@ -5386,8 +5674,26 @@
       <c r="CC18">
         <v>0.99389802858021203</v>
       </c>
+      <c r="CD18">
+        <v>423.16708229426399</v>
+      </c>
+      <c r="CE18">
+        <v>890.57142857142901</v>
+      </c>
+      <c r="CF18">
+        <v>1367.5</v>
+      </c>
+      <c r="CG18">
+        <v>430</v>
+      </c>
+      <c r="CH18">
+        <v>1020</v>
+      </c>
+      <c r="CI18">
+        <v>1450</v>
+      </c>
     </row>
-    <row r="19" spans="1:81">
+    <row r="19" spans="1:87">
       <c r="A19">
         <v>19</v>
       </c>
@@ -5515,7 +5821,7 @@
         <v>0.320175438596491</v>
       </c>
     </row>
-    <row r="20" spans="1:81">
+    <row r="20" spans="1:87">
       <c r="A20">
         <v>20</v>
       </c>
@@ -5643,7 +5949,7 @@
         <v>0.31034482758620702</v>
       </c>
     </row>
-    <row r="21" spans="1:81">
+    <row r="21" spans="1:87">
       <c r="A21">
         <v>21</v>
       </c>
@@ -5886,6 +6192,24 @@
       </c>
       <c r="CC21">
         <v>0.98437077575726295</v>
+      </c>
+      <c r="CD21">
+        <v>580.12068965517199</v>
+      </c>
+      <c r="CE21">
+        <v>890.47619047619003</v>
+      </c>
+      <c r="CF21">
+        <v>1050.125</v>
+      </c>
+      <c r="CG21">
+        <v>650</v>
+      </c>
+      <c r="CH21">
+        <v>975</v>
+      </c>
+      <c r="CI21">
+        <v>1174.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
characterized gen/sf richness patterns, made fig 3
</commit_message>
<xml_diff>
--- a/Sheets/datasetOverview.xlsx
+++ b/Sheets/datasetOverview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="-140" yWindow="0" windowWidth="34100" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="271">
   <si>
     <t>ID</t>
   </si>
@@ -790,6 +790,48 @@
   </si>
   <si>
     <t>sp.seRng.2000</t>
+  </si>
+  <si>
+    <t>genPatt</t>
+  </si>
+  <si>
+    <t>sfPatt</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>LPMP</t>
+  </si>
+  <si>
+    <t>GenPk</t>
+  </si>
+  <si>
+    <t>GenMax</t>
+  </si>
+  <si>
+    <t>GenBase</t>
+  </si>
+  <si>
+    <t>GenPerc</t>
+  </si>
+  <si>
+    <t>GenPkBase</t>
+  </si>
+  <si>
+    <t>SFPk</t>
+  </si>
+  <si>
+    <t>SFMax</t>
+  </si>
+  <si>
+    <t>SFBase</t>
+  </si>
+  <si>
+    <t>SFPerc</t>
+  </si>
+  <si>
+    <t>SFPkBase</t>
   </si>
 </sst>
 </file>
@@ -1275,13 +1317,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DD21"/>
+  <dimension ref="A1:DR21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="CN2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <pane xSplit="10" ySplit="1" topLeftCell="DE2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CY9" sqref="CY9:CY11"/>
+      <selection pane="bottomRight" activeCell="DR21" sqref="A1:DR21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1292,7 +1334,7 @@
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108">
+    <row r="1" spans="1:122">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1617,8 +1659,50 @@
       <c r="DD1" t="s">
         <v>253</v>
       </c>
+      <c r="DE1" t="s">
+        <v>257</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>258</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>25</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>261</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>262</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>263</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>264</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>265</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>26</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>266</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>267</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>268</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>269</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>270</v>
+      </c>
     </row>
-    <row r="2" spans="1:108">
+    <row r="2" spans="1:122">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1943,8 +2027,50 @@
       <c r="DD2">
         <v>1432.8</v>
       </c>
+      <c r="DE2" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>145</v>
+      </c>
+      <c r="DG2">
+        <v>40</v>
+      </c>
+      <c r="DH2">
+        <v>1800</v>
+      </c>
+      <c r="DI2">
+        <v>28</v>
+      </c>
+      <c r="DJ2">
+        <v>15</v>
+      </c>
+      <c r="DK2">
+        <v>1.86666666666667</v>
+      </c>
+      <c r="DL2">
+        <v>782</v>
+      </c>
+      <c r="DM2">
+        <v>6</v>
+      </c>
+      <c r="DN2">
+        <v>1800</v>
+      </c>
+      <c r="DO2">
+        <v>6</v>
+      </c>
+      <c r="DP2">
+        <v>4</v>
+      </c>
+      <c r="DQ2">
+        <v>1.5</v>
+      </c>
+      <c r="DR2">
+        <v>782</v>
+      </c>
     </row>
-    <row r="3" spans="1:108">
+    <row r="3" spans="1:122">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2269,8 +2395,50 @@
       <c r="DD3">
         <v>1798.9295999999999</v>
       </c>
+      <c r="DE3" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF3" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG3">
+        <v>23</v>
+      </c>
+      <c r="DH3">
+        <v>1300</v>
+      </c>
+      <c r="DI3">
+        <v>22</v>
+      </c>
+      <c r="DJ3">
+        <v>9</v>
+      </c>
+      <c r="DK3">
+        <v>2.4444444444444402</v>
+      </c>
+      <c r="DL3">
+        <v>636</v>
+      </c>
+      <c r="DM3">
+        <v>5</v>
+      </c>
+      <c r="DN3">
+        <v>800</v>
+      </c>
+      <c r="DO3">
+        <v>4</v>
+      </c>
+      <c r="DP3">
+        <v>3</v>
+      </c>
+      <c r="DQ3">
+        <v>1.3333333333333299</v>
+      </c>
+      <c r="DR3">
+        <v>136</v>
+      </c>
     </row>
-    <row r="4" spans="1:108">
+    <row r="4" spans="1:122">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2595,8 +2763,50 @@
       <c r="DD4">
         <v>1840</v>
       </c>
+      <c r="DE4" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF4" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG4">
+        <v>35</v>
+      </c>
+      <c r="DH4">
+        <v>700</v>
+      </c>
+      <c r="DI4">
+        <v>27</v>
+      </c>
+      <c r="DJ4">
+        <v>15</v>
+      </c>
+      <c r="DK4">
+        <v>1.8</v>
+      </c>
+      <c r="DL4">
+        <v>575</v>
+      </c>
+      <c r="DM4">
+        <v>5</v>
+      </c>
+      <c r="DN4">
+        <v>100</v>
+      </c>
+      <c r="DO4">
+        <v>5</v>
+      </c>
+      <c r="DP4">
+        <v>5</v>
+      </c>
+      <c r="DQ4">
+        <v>1</v>
+      </c>
+      <c r="DR4">
+        <v>-25</v>
+      </c>
     </row>
-    <row r="5" spans="1:108">
+    <row r="5" spans="1:122">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2879,8 +3089,50 @@
       <c r="CP5">
         <v>650</v>
       </c>
+      <c r="DE5" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF5" t="s">
+        <v>145</v>
+      </c>
+      <c r="DG5">
+        <v>29</v>
+      </c>
+      <c r="DH5">
+        <v>1400</v>
+      </c>
+      <c r="DI5">
+        <v>23</v>
+      </c>
+      <c r="DJ5">
+        <v>2</v>
+      </c>
+      <c r="DK5">
+        <v>11.5</v>
+      </c>
+      <c r="DL5">
+        <v>748</v>
+      </c>
+      <c r="DM5">
+        <v>8</v>
+      </c>
+      <c r="DN5">
+        <v>1400</v>
+      </c>
+      <c r="DO5">
+        <v>6</v>
+      </c>
+      <c r="DP5">
+        <v>1</v>
+      </c>
+      <c r="DQ5">
+        <v>6</v>
+      </c>
+      <c r="DR5">
+        <v>748</v>
+      </c>
     </row>
-    <row r="6" spans="1:108">
+    <row r="6" spans="1:122">
       <c r="A6">
         <v>6</v>
       </c>
@@ -3205,8 +3457,50 @@
       <c r="DD6">
         <v>1802.7200107000001</v>
       </c>
+      <c r="DE6" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF6" t="s">
+        <v>145</v>
+      </c>
+      <c r="DG6">
+        <v>28</v>
+      </c>
+      <c r="DH6">
+        <v>1400</v>
+      </c>
+      <c r="DI6">
+        <v>23</v>
+      </c>
+      <c r="DJ6">
+        <v>4</v>
+      </c>
+      <c r="DK6">
+        <v>5.75</v>
+      </c>
+      <c r="DL6">
+        <v>1262</v>
+      </c>
+      <c r="DM6">
+        <v>5</v>
+      </c>
+      <c r="DN6">
+        <v>1000</v>
+      </c>
+      <c r="DO6">
+        <v>4</v>
+      </c>
+      <c r="DP6">
+        <v>2</v>
+      </c>
+      <c r="DQ6">
+        <v>2</v>
+      </c>
+      <c r="DR6">
+        <v>862</v>
+      </c>
     </row>
-    <row r="7" spans="1:108">
+    <row r="7" spans="1:122">
       <c r="A7">
         <v>7</v>
       </c>
@@ -3334,7 +3628,7 @@
         <v>0.43595422665190098</v>
       </c>
     </row>
-    <row r="8" spans="1:108">
+    <row r="8" spans="1:122">
       <c r="A8">
         <v>8</v>
       </c>
@@ -3638,8 +3932,50 @@
       <c r="CW8">
         <v>987.5</v>
       </c>
+      <c r="DE8" t="s">
+        <v>147</v>
+      </c>
+      <c r="DF8" t="s">
+        <v>147</v>
+      </c>
+      <c r="DG8">
+        <v>20</v>
+      </c>
+      <c r="DH8">
+        <v>250</v>
+      </c>
+      <c r="DI8">
+        <v>13</v>
+      </c>
+      <c r="DJ8">
+        <v>13</v>
+      </c>
+      <c r="DK8">
+        <v>1</v>
+      </c>
+      <c r="DL8">
+        <v>250</v>
+      </c>
+      <c r="DM8">
+        <v>4</v>
+      </c>
+      <c r="DN8">
+        <v>250</v>
+      </c>
+      <c r="DO8">
+        <v>4</v>
+      </c>
+      <c r="DP8">
+        <v>4</v>
+      </c>
+      <c r="DQ8">
+        <v>1</v>
+      </c>
+      <c r="DR8">
+        <v>250</v>
+      </c>
     </row>
-    <row r="9" spans="1:108">
+    <row r="9" spans="1:122">
       <c r="A9">
         <v>9</v>
       </c>
@@ -3964,8 +4300,50 @@
       <c r="DD9">
         <v>1750</v>
       </c>
+      <c r="DE9" t="s">
+        <v>260</v>
+      </c>
+      <c r="DF9" t="s">
+        <v>260</v>
+      </c>
+      <c r="DG9">
+        <v>28</v>
+      </c>
+      <c r="DH9">
+        <v>425</v>
+      </c>
+      <c r="DI9">
+        <v>26</v>
+      </c>
+      <c r="DJ9">
+        <v>21</v>
+      </c>
+      <c r="DK9">
+        <v>1.2380952380952399</v>
+      </c>
+      <c r="DL9">
+        <v>425</v>
+      </c>
+      <c r="DM9">
+        <v>8</v>
+      </c>
+      <c r="DN9">
+        <v>425</v>
+      </c>
+      <c r="DO9">
+        <v>8</v>
+      </c>
+      <c r="DP9">
+        <v>7</v>
+      </c>
+      <c r="DQ9">
+        <v>1.1428571428571399</v>
+      </c>
+      <c r="DR9">
+        <v>425</v>
+      </c>
     </row>
-    <row r="10" spans="1:108">
+    <row r="10" spans="1:122">
       <c r="A10">
         <v>10</v>
       </c>
@@ -4227,8 +4605,50 @@
       <c r="CI10">
         <v>550</v>
       </c>
+      <c r="DE10" t="s">
+        <v>146</v>
+      </c>
+      <c r="DF10" t="s">
+        <v>147</v>
+      </c>
+      <c r="DG10">
+        <v>15</v>
+      </c>
+      <c r="DH10">
+        <v>800</v>
+      </c>
+      <c r="DI10">
+        <v>12</v>
+      </c>
+      <c r="DJ10">
+        <v>12</v>
+      </c>
+      <c r="DK10">
+        <v>1</v>
+      </c>
+      <c r="DL10">
+        <v>322</v>
+      </c>
+      <c r="DM10">
+        <v>6</v>
+      </c>
+      <c r="DN10">
+        <v>800</v>
+      </c>
+      <c r="DO10">
+        <v>6</v>
+      </c>
+      <c r="DP10">
+        <v>6</v>
+      </c>
+      <c r="DQ10">
+        <v>1</v>
+      </c>
+      <c r="DR10">
+        <v>322</v>
+      </c>
     </row>
-    <row r="11" spans="1:108">
+    <row r="11" spans="1:122">
       <c r="A11">
         <v>11</v>
       </c>
@@ -4553,8 +4973,50 @@
       <c r="DD11">
         <v>1195.5</v>
       </c>
+      <c r="DE11" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF11" t="s">
+        <v>145</v>
+      </c>
+      <c r="DG11">
+        <v>24</v>
+      </c>
+      <c r="DH11">
+        <v>800</v>
+      </c>
+      <c r="DI11">
+        <v>16</v>
+      </c>
+      <c r="DJ11">
+        <v>2</v>
+      </c>
+      <c r="DK11">
+        <v>8</v>
+      </c>
+      <c r="DL11">
+        <v>609</v>
+      </c>
+      <c r="DM11">
+        <v>4</v>
+      </c>
+      <c r="DN11">
+        <v>600</v>
+      </c>
+      <c r="DO11">
+        <v>4</v>
+      </c>
+      <c r="DP11">
+        <v>1</v>
+      </c>
+      <c r="DQ11">
+        <v>4</v>
+      </c>
+      <c r="DR11">
+        <v>409</v>
+      </c>
     </row>
-    <row r="12" spans="1:108">
+    <row r="12" spans="1:122">
       <c r="A12">
         <v>12</v>
       </c>
@@ -4682,7 +5144,7 @@
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:108">
+    <row r="13" spans="1:122">
       <c r="A13">
         <v>13</v>
       </c>
@@ -5007,8 +5469,50 @@
       <c r="DD13">
         <v>1150</v>
       </c>
+      <c r="DE13" t="s">
+        <v>147</v>
+      </c>
+      <c r="DF13" t="s">
+        <v>147</v>
+      </c>
+      <c r="DG13">
+        <v>17</v>
+      </c>
+      <c r="DH13">
+        <v>400</v>
+      </c>
+      <c r="DI13">
+        <v>14</v>
+      </c>
+      <c r="DJ13">
+        <v>14</v>
+      </c>
+      <c r="DK13">
+        <v>1</v>
+      </c>
+      <c r="DL13">
+        <v>12</v>
+      </c>
+      <c r="DM13">
+        <v>4</v>
+      </c>
+      <c r="DN13">
+        <v>400</v>
+      </c>
+      <c r="DO13">
+        <v>4</v>
+      </c>
+      <c r="DP13">
+        <v>4</v>
+      </c>
+      <c r="DQ13">
+        <v>1</v>
+      </c>
+      <c r="DR13">
+        <v>12</v>
+      </c>
     </row>
-    <row r="14" spans="1:108">
+    <row r="14" spans="1:122">
       <c r="A14">
         <v>14</v>
       </c>
@@ -5312,8 +5816,50 @@
       <c r="CW14">
         <v>856.5</v>
       </c>
+      <c r="DE14" t="s">
+        <v>146</v>
+      </c>
+      <c r="DF14" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG14">
+        <v>20</v>
+      </c>
+      <c r="DH14">
+        <v>440</v>
+      </c>
+      <c r="DI14">
+        <v>16</v>
+      </c>
+      <c r="DJ14">
+        <v>10</v>
+      </c>
+      <c r="DK14">
+        <v>1.6</v>
+      </c>
+      <c r="DL14">
+        <v>222</v>
+      </c>
+      <c r="DM14">
+        <v>6</v>
+      </c>
+      <c r="DN14">
+        <v>511</v>
+      </c>
+      <c r="DO14">
+        <v>6</v>
+      </c>
+      <c r="DP14">
+        <v>4</v>
+      </c>
+      <c r="DQ14">
+        <v>1.5</v>
+      </c>
+      <c r="DR14">
+        <v>293</v>
+      </c>
     </row>
-    <row r="15" spans="1:108">
+    <row r="15" spans="1:122">
       <c r="A15">
         <v>15</v>
       </c>
@@ -5638,8 +6184,50 @@
       <c r="DD15">
         <v>1350</v>
       </c>
+      <c r="DE15" t="s">
+        <v>145</v>
+      </c>
+      <c r="DF15" t="s">
+        <v>145</v>
+      </c>
+      <c r="DG15">
+        <v>18</v>
+      </c>
+      <c r="DH15">
+        <v>1000</v>
+      </c>
+      <c r="DI15">
+        <v>17</v>
+      </c>
+      <c r="DJ15">
+        <v>9</v>
+      </c>
+      <c r="DK15">
+        <v>1.8888888888888899</v>
+      </c>
+      <c r="DL15">
+        <v>1000</v>
+      </c>
+      <c r="DM15">
+        <v>5</v>
+      </c>
+      <c r="DN15">
+        <v>1000</v>
+      </c>
+      <c r="DO15">
+        <v>5</v>
+      </c>
+      <c r="DP15">
+        <v>4</v>
+      </c>
+      <c r="DQ15">
+        <v>1.25</v>
+      </c>
+      <c r="DR15">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="16" spans="1:108">
+    <row r="16" spans="1:122">
       <c r="A16">
         <v>16</v>
       </c>
@@ -5901,8 +6489,50 @@
       <c r="CI16">
         <v>800</v>
       </c>
+      <c r="DE16" t="s">
+        <v>147</v>
+      </c>
+      <c r="DF16" t="s">
+        <v>259</v>
+      </c>
+      <c r="DG16">
+        <v>57</v>
+      </c>
+      <c r="DH16">
+        <v>300</v>
+      </c>
+      <c r="DI16">
+        <v>49</v>
+      </c>
+      <c r="DJ16">
+        <v>49</v>
+      </c>
+      <c r="DK16">
+        <v>1</v>
+      </c>
+      <c r="DL16">
+        <v>300</v>
+      </c>
+      <c r="DM16">
+        <v>10</v>
+      </c>
+      <c r="DN16">
+        <v>300</v>
+      </c>
+      <c r="DO16">
+        <v>10</v>
+      </c>
+      <c r="DP16">
+        <v>10</v>
+      </c>
+      <c r="DQ16">
+        <v>1</v>
+      </c>
+      <c r="DR16">
+        <v>300</v>
+      </c>
     </row>
-    <row r="17" spans="1:108">
+    <row r="17" spans="1:122">
       <c r="A17">
         <v>17</v>
       </c>
@@ -6227,8 +6857,50 @@
       <c r="DD17">
         <v>1100</v>
       </c>
+      <c r="DE17" t="s">
+        <v>147</v>
+      </c>
+      <c r="DF17" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG17">
+        <v>28</v>
+      </c>
+      <c r="DH17">
+        <v>100</v>
+      </c>
+      <c r="DI17">
+        <v>24</v>
+      </c>
+      <c r="DJ17">
+        <v>24</v>
+      </c>
+      <c r="DK17">
+        <v>1</v>
+      </c>
+      <c r="DL17">
+        <v>100</v>
+      </c>
+      <c r="DM17">
+        <v>5</v>
+      </c>
+      <c r="DN17">
+        <v>200</v>
+      </c>
+      <c r="DO17">
+        <v>5</v>
+      </c>
+      <c r="DP17">
+        <v>4</v>
+      </c>
+      <c r="DQ17">
+        <v>1.25</v>
+      </c>
+      <c r="DR17">
+        <v>200</v>
+      </c>
     </row>
-    <row r="18" spans="1:108">
+    <row r="18" spans="1:122">
       <c r="A18">
         <v>18</v>
       </c>
@@ -6553,8 +7225,50 @@
       <c r="DD18">
         <v>1450</v>
       </c>
+      <c r="DE18" t="s">
+        <v>146</v>
+      </c>
+      <c r="DF18" t="s">
+        <v>147</v>
+      </c>
+      <c r="DG18">
+        <v>70</v>
+      </c>
+      <c r="DH18">
+        <v>300</v>
+      </c>
+      <c r="DI18">
+        <v>61</v>
+      </c>
+      <c r="DJ18">
+        <v>58</v>
+      </c>
+      <c r="DK18">
+        <v>1.05172413793103</v>
+      </c>
+      <c r="DL18">
+        <v>300</v>
+      </c>
+      <c r="DM18">
+        <v>12</v>
+      </c>
+      <c r="DN18">
+        <v>50</v>
+      </c>
+      <c r="DO18">
+        <v>12</v>
+      </c>
+      <c r="DP18">
+        <v>12</v>
+      </c>
+      <c r="DQ18">
+        <v>1</v>
+      </c>
+      <c r="DR18">
+        <v>50</v>
+      </c>
     </row>
-    <row r="19" spans="1:108">
+    <row r="19" spans="1:122">
       <c r="A19">
         <v>19</v>
       </c>
@@ -6682,7 +7396,7 @@
         <v>0.320175438596491</v>
       </c>
     </row>
-    <row r="20" spans="1:108">
+    <row r="20" spans="1:122">
       <c r="A20">
         <v>20</v>
       </c>
@@ -6810,7 +7524,7 @@
         <v>0.31034482758620702</v>
       </c>
     </row>
-    <row r="21" spans="1:108">
+    <row r="21" spans="1:122">
       <c r="A21">
         <v>21</v>
       </c>
@@ -7072,8 +7786,53 @@
       <c r="CI21">
         <v>1174.5</v>
       </c>
+      <c r="DE21" t="s">
+        <v>260</v>
+      </c>
+      <c r="DF21" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG21">
+        <v>42</v>
+      </c>
+      <c r="DH21">
+        <v>300</v>
+      </c>
+      <c r="DI21">
+        <v>39</v>
+      </c>
+      <c r="DJ21">
+        <v>36</v>
+      </c>
+      <c r="DK21">
+        <v>1.0833333333333299</v>
+      </c>
+      <c r="DL21">
+        <v>300</v>
+      </c>
+      <c r="DM21">
+        <v>7</v>
+      </c>
+      <c r="DN21">
+        <v>200</v>
+      </c>
+      <c r="DO21">
+        <v>7</v>
+      </c>
+      <c r="DP21">
+        <v>6</v>
+      </c>
+      <c r="DQ21">
+        <v>1.1666666666666701</v>
+      </c>
+      <c r="DR21">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:DR21">
+    <sortCondition ref="D2:D21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>